<commit_message>
actualizacion de py que genera la correlacion cramer V para las variables categoricas
</commit_message>
<xml_diff>
--- a/misc/catalogos/catalogo_1.xlsx
+++ b/misc/catalogos/catalogo_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yeimunoz\Documents\caramelo\catalogos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0EC8C5-532C-4C93-BFFC-5C6A01E0A472}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57E8FE6-3AC4-4D20-98BA-F29EFC909B54}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{855AF920-00D3-496D-A6BC-53AC25B09997}"/>
   </bookViews>
@@ -36,162 +36,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="500">
   <si>
-    <t>La organización se destaca ante la sociedad en los campos más significativos de su trabajo</t>
-  </si>
-  <si>
-    <t>En la organización cooperamos cuando las personas cometen errores</t>
-  </si>
-  <si>
-    <t>Tenemos mucho trabajo por delante para ganar conciencia ecológica en la organización</t>
-  </si>
-  <si>
-    <t>La organización es considerada una organización influyente y con buenas conexiones</t>
-  </si>
-  <si>
-    <t>Cada persona de la organización está comprometida con los resultados</t>
-  </si>
-  <si>
-    <t>La organización suele ayudar a las causas sociales y situaciones de crisis que se presentan</t>
-  </si>
-  <si>
-    <t>Con frecuencia las decisiones de la organización ponen en riesgo su continuidad en el futuro</t>
-  </si>
-  <si>
-    <t>La organización se mueve despacio. Prefiere no tomar riesgos y cuida mucho su prestigio</t>
-  </si>
-  <si>
-    <t>Los espacios de la organización son confortable y me aporta lo que necesito para estar bien</t>
-  </si>
-  <si>
-    <t>La organización es principalmente conservadora y clásica</t>
-  </si>
-  <si>
-    <t>Me siento cómodo en esta cultura y entorno organizacional</t>
-  </si>
-  <si>
-    <t>Trabajar aquí me hace sentir bienestar. Me siento protegido y tranquilo</t>
-  </si>
-  <si>
-    <t>Cada equipo tiene sus propios retos y resultados. En esta organización todos somos muy distintos y poco interactuamos entre áreas distintas</t>
-  </si>
-  <si>
-    <t>Todos los que van llegando nuevos a la organización se adaptan a la cultura y se ajustan a las maneras en que aquí se hacen las cosas</t>
-  </si>
-  <si>
-    <t>Tenemos serios problemas de comunicación: no tenemos espacios para escucharnos y no siempre nos enteramos de lo que pasa</t>
-  </si>
-  <si>
     <t>Las celebraciones de la empresa nos permiten integrarnos y pasar un tiempo juntos</t>
   </si>
   <si>
     <t>El trabajo en equipo caracteriza nuestra forma de hacer las cosas</t>
   </si>
   <si>
-    <t>La imagen que se percibe de la organización se corresponde con lo que yo vivo como colaborador</t>
-  </si>
-  <si>
     <t>Ocasionalmente se reconocen los aportes de las personas.</t>
   </si>
   <si>
-    <t>Los espacios formales de retroalimentación son pocos y podrían ser más productivos</t>
-  </si>
-  <si>
-    <t>En la organización tengo la oportunidad de mejorar mis habilidades</t>
-  </si>
-  <si>
-    <t>Pedir ayuda es poco habitual en nuestra organización</t>
-  </si>
-  <si>
-    <t>Mi familia y amigos se sienten orgullosos de que yo trabaje aquí</t>
-  </si>
-  <si>
-    <t>Las maneras actuales de priorizar y actuar en la organización nos están acercando al propósito y plan estratégico trazado</t>
-  </si>
-  <si>
-    <t>Los planes y proyectos nuevos de la organización se acompasan y conectan con el ritmo del equipo y sus planes previamente trazados</t>
-  </si>
-  <si>
-    <t>Me inspira la misión y propósito de la organización</t>
-  </si>
-  <si>
-    <t>La organización se destaca por obtener resultados excepcionales en todo lo que hace.</t>
-  </si>
-  <si>
-    <t>En la organización se siente el colegaje y amistad tanto cuando cometemos errores como cuando obtenemos buenos resultados</t>
-  </si>
-  <si>
-    <t>La organización se destaca por sus prácticas medioambientales y de sostenibilidad</t>
-  </si>
-  <si>
-    <t>La organización trabaja en red y colabora con muchas otras organizaciones y personas. Esto nos enriquece a todos</t>
-  </si>
-  <si>
-    <t>En esta organización se premia la proactividad y quienes se destacan suelen ser promovidos a nuevos retos</t>
-  </si>
-  <si>
-    <t>Nuestra organización se destaca por su contribución a la sociedad</t>
-  </si>
-  <si>
-    <t>Las decisiones que ha tomado la organización en el último año nos llevarán más lejos y están alineadas a los objetivos</t>
-  </si>
-  <si>
-    <t>La organización incorpora cambios con agilidad y capacidad de adaptación</t>
-  </si>
-  <si>
-    <t>Los espacios de esta organización son excepcionales</t>
-  </si>
-  <si>
-    <t>Uno de los atributos más visibles de nuestra organización es la innovación</t>
-  </si>
-  <si>
     <t>Recomiendo este lugar como una gran empresa para trabajar</t>
   </si>
   <si>
-    <t>En la organización se respira un ambiente de tranquilidad y armonía</t>
-  </si>
-  <si>
-    <t>En esta organización los espacios para conversar y escuchar son frecuentes y valorados</t>
-  </si>
-  <si>
-    <t>Las personas que trabajan en la organización imprimen sus propias cualidades en la cultura y la enriquecen</t>
-  </si>
-  <si>
-    <t>Somos una organización con buena comunicación: escuchamos y somos escuchados y sabemos lo que pasa</t>
-  </si>
-  <si>
-    <t>En la organización celebramos los logros y aprendizajes</t>
-  </si>
-  <si>
-    <t>Confío en los líderes de la organización</t>
-  </si>
-  <si>
-    <t>Me gusta la personalidad de esta organización. Proyecta confianza y es afín a mi estilo de vida</t>
-  </si>
-  <si>
-    <t>Mis resultados son reconocidos y valorados por la organización</t>
-  </si>
-  <si>
-    <t>Retroalimentar el trabajo propio y de los demás para aprender juntos es un hábito de nuestra organización</t>
-  </si>
-  <si>
-    <t>En la organización todos contribuimos de manera destacada</t>
-  </si>
-  <si>
-    <t>En la organización las personas pedimos ayuda, la ofrecemos y la recibimos de parte de otros compañeros</t>
-  </si>
-  <si>
-    <t>Me siento orgulloso de ser parte del equipo humano de esta organización</t>
-  </si>
-  <si>
-    <t>El propósito de la organización me impulsa y saca lo mejor de mi</t>
-  </si>
-  <si>
-    <t>La organización propicia un sano equilibrio vida/trabajo</t>
-  </si>
-  <si>
-    <t>Los valores que promueve la organización corresponden con los míos</t>
-  </si>
-  <si>
     <t>En nuestro equipo logramos las metas que nos proponemos</t>
   </si>
   <si>
@@ -204,42 +60,21 @@
     <t>Tengo amigos en mi equipo de trabajo directo</t>
   </si>
   <si>
-    <t>El líder es claro y asigna las tareas a cada persona para lograr los objetivos del equipo</t>
-  </si>
-  <si>
     <t>Nuestro equipo participa poco en temas sociales</t>
   </si>
   <si>
-    <t>Sé que hace cada persona de mi equipo. Les puedo ayudar y puedo contar con mis pares cuando necesito ayuda</t>
-  </si>
-  <si>
     <t>Mi equipo es bastante estable y las actividades que desarrollamos ya las conocemos bastante bien y funcionan como un relojito</t>
   </si>
   <si>
     <t>El lugar de trabajo de mi equipo es adecuado para cumplir los objetivos</t>
   </si>
   <si>
-    <t>El proceso de nuestra área no suele tener muchas innovaciones</t>
-  </si>
-  <si>
-    <t>Los procesos y procedimientos están muy claros y es indispensable seguirlos al pie de la letra</t>
-  </si>
-  <si>
-    <t>Yo me aseguro de no ser un problema para los demás. Otros deberían hacer lo mismo</t>
-  </si>
-  <si>
     <t>La alta operatividad de nuestro rol limita los espacios para conversar pero esto no es fundamental en lo que hacemos</t>
   </si>
   <si>
     <t>Destinamos tiempo para aportar en los procesos del equipo y enriquecer conjuntamente el norte de lo que hacemos.</t>
   </si>
   <si>
-    <t>La comunicación del equipo nos acerca como personas y facilita nuestros resultados</t>
-  </si>
-  <si>
-    <t>El líder propicia espacios de encuentro y compartir como equipo</t>
-  </si>
-  <si>
     <t>Mi lider directo es claro y me ayuda a lograr los retos de mi trabajo</t>
   </si>
   <si>
@@ -249,36 +84,9 @@
     <t>Cada colaborador conoce cual es su rol dentro del equipo y se valora que lo haga bien</t>
   </si>
   <si>
-    <t>Todos somos responsables de monitorear los riesgos del área</t>
-  </si>
-  <si>
-    <t>Considero que mis pares están abiertos a recibir opiniones diferentes a las suyas</t>
-  </si>
-  <si>
-    <t>En el equipo cada uno sabe su tarea y es fundamental favorecer su concentración para que la logre</t>
-  </si>
-  <si>
-    <t>Mi relación con mi jefe inmediato se basa en el respeto y la claridad</t>
-  </si>
-  <si>
-    <t>Mi plan de carrera tiene futuro si permanezco en esta organización</t>
-  </si>
-  <si>
-    <t>Tengo acceso a la información y recursos necesarios para realizar mi trabajo</t>
-  </si>
-  <si>
     <t>El ambiente de trabajo del equipo refleja la cultura organizacional que se predica</t>
   </si>
   <si>
-    <t>Mi líder es claro con las metas y despliega incentivos claros para motivar resultados más allá de lo esperado</t>
-  </si>
-  <si>
-    <t>Siento el respaldo de mi líder, incluso cuando cometo errores</t>
-  </si>
-  <si>
-    <t>En nuestro equipo le damos mucho valor a la conciencia ecológica y se evidencia en las pequeñas decisiones cotidianas</t>
-  </si>
-  <si>
     <t>Yo colaboro con mis compañeros y ellos colaboran conmigo para lograr los resultados</t>
   </si>
   <si>
@@ -288,24 +96,12 @@
     <t>Mi lider directo es sensible socialmente y nos involucra en temas sociales</t>
   </si>
   <si>
-    <t>Mi jefe es justo, claro y profesional para tomar decisiones. Confío en su criterio</t>
-  </si>
-  <si>
     <t>En nuestro equipo estamos habituados a los cambios y se nos facilita hacer cosas nuevas o diferentes</t>
   </si>
   <si>
     <t>Nuestro espacio de trabajo -oficinas, salones y espacios - favorece un buen ambiente para trabajar y compartir</t>
   </si>
   <si>
-    <t>Estoy involucrado en el seguimiento de innovaciones y nuevos proyectos del área</t>
-  </si>
-  <si>
-    <t>Tengo libertad para decidir cómo realizar mi trabajo</t>
-  </si>
-  <si>
-    <t>Con mi equipo inmediato me siento en un entorno saludable física y emocionalmente</t>
-  </si>
-  <si>
     <t>Me siento escuchado por mi jefe y mis aportes son tenidos en cuenta para mejorar el trabajo de todos</t>
   </si>
   <si>
@@ -318,18 +114,9 @@
     <t>En el equipo tenemos frecuentes espacios para compartir logros, avances, resultados y retos personales y profesionales</t>
   </si>
   <si>
-    <t>En nuestro equipo todos aportamos y el líder nos acompaña y direcciona para lograr resultados superiores a los esperados</t>
-  </si>
-  <si>
-    <t>Entiendo claramente mi rol y aporte a los resultados del equipo y de la organización</t>
-  </si>
-  <si>
     <t>Recibo reconocimiento de mi jefe inmediato que me motiva a seguir destacandome por mi trabajo</t>
   </si>
   <si>
-    <t>Recibo retroalimentación de mi jefe inmediato que me permite mejorar permanentemente</t>
-  </si>
-  <si>
     <t>Puedo poner mi creatividad y talentos personales en el desempeño de mi trabajo</t>
   </si>
   <si>
@@ -339,18 +126,9 @@
     <t>Estoy orgullosa de mi jefe</t>
   </si>
   <si>
-    <t>Tengo claras oportunidades de crecer dentro de mi equipo y de la organización</t>
-  </si>
-  <si>
-    <t>La dinámica de mi equipo de trabajo me permite experimentar un sano equilibrio entre la vida laboral y la vida personal</t>
-  </si>
-  <si>
     <t>En nuestro equipo cada persona puede desplegar todo su talento al servicio del equipo y los resultados</t>
   </si>
   <si>
-    <t xml:space="preserve">Con cuál de las siguientes afirmaciones te identificas más? </t>
-  </si>
-  <si>
     <t>Inversa</t>
   </si>
   <si>
@@ -1146,27 +924,15 @@
     <t>id_pnt</t>
   </si>
   <si>
-    <t>Conexión yo</t>
-  </si>
-  <si>
     <t>Equilibrio yo</t>
   </si>
   <si>
-    <t>Propósito yo</t>
-  </si>
-  <si>
     <t>Orgullo (eNps) yo</t>
   </si>
   <si>
     <t>Pedir ayuda yo</t>
   </si>
   <si>
-    <t>Contribución yo</t>
-  </si>
-  <si>
-    <t>Retroalimentación yo</t>
-  </si>
-  <si>
     <t>Reconocimiento yo</t>
   </si>
   <si>
@@ -1179,12 +945,6 @@
     <t>Rituales yo</t>
   </si>
   <si>
-    <t>Comunicación yo</t>
-  </si>
-  <si>
-    <t>Contribución individual a la cultura yo</t>
-  </si>
-  <si>
     <t>Conversaciones yo</t>
   </si>
   <si>
@@ -1194,12 +954,6 @@
     <t>Relevancia yo</t>
   </si>
   <si>
-    <t>Innovación yo</t>
-  </si>
-  <si>
-    <t>Espacios físicos aliados de la cultura yo</t>
-  </si>
-  <si>
     <t>Adaptabilidad yo</t>
   </si>
   <si>
@@ -1218,33 +972,18 @@
     <t>Conciencia Sostenible yo</t>
   </si>
   <si>
-    <t>Servir con cercanía yo</t>
-  </si>
-  <si>
     <t>Superar metas yo</t>
   </si>
   <si>
-    <t>Conexión nosotros 1</t>
-  </si>
-  <si>
     <t>Equilibrio nosotros 1</t>
   </si>
   <si>
-    <t>Propósito nosotros 1</t>
-  </si>
-  <si>
     <t>Orgullo (eNps) nosotros 1</t>
   </si>
   <si>
     <t>Pedir ayuda nosotros 1</t>
   </si>
   <si>
-    <t>Contribución nosotros 1</t>
-  </si>
-  <si>
-    <t>Retroalimentación nosotros 1</t>
-  </si>
-  <si>
     <t>Reconocimiento nosotros 1</t>
   </si>
   <si>
@@ -1257,12 +996,6 @@
     <t>Rituales nosotros 1</t>
   </si>
   <si>
-    <t>Comunicación nosotros 1</t>
-  </si>
-  <si>
-    <t>Contribución individual a la cultura nosotros 1</t>
-  </si>
-  <si>
     <t>Conversaciones nosotros 1</t>
   </si>
   <si>
@@ -1272,12 +1005,6 @@
     <t>Relevancia nosotros 1</t>
   </si>
   <si>
-    <t>Innovación nosotros 1</t>
-  </si>
-  <si>
-    <t>Espacios físicos aliados de la cultura nosotros 1</t>
-  </si>
-  <si>
     <t>Adaptabilidad nosotros 1</t>
   </si>
   <si>
@@ -1296,33 +1023,18 @@
     <t>Conciencia Sostenible nosotros 1</t>
   </si>
   <si>
-    <t>Servir con cercanía nosotros 1</t>
-  </si>
-  <si>
     <t>Superar metas nosotros 1</t>
   </si>
   <si>
-    <t>Conexión nosotros 2</t>
-  </si>
-  <si>
     <t>Equilibrio nosotros 2</t>
   </si>
   <si>
-    <t>Propósito nosotros 2</t>
-  </si>
-  <si>
     <t>Orgullo (eNps) nosotros 2</t>
   </si>
   <si>
     <t>Pedir ayuda nosotros 2</t>
   </si>
   <si>
-    <t>Contribución nosotros 2</t>
-  </si>
-  <si>
-    <t>Retroalimentación nosotros 2</t>
-  </si>
-  <si>
     <t>Reconocimiento nosotros 2</t>
   </si>
   <si>
@@ -1335,12 +1047,6 @@
     <t>Rituales nosotros 2</t>
   </si>
   <si>
-    <t>Comunicación nosotros 2</t>
-  </si>
-  <si>
-    <t>Contribución individual a la cultura nosotros 2</t>
-  </si>
-  <si>
     <t>Conversaciones nosotros 2</t>
   </si>
   <si>
@@ -1350,12 +1056,6 @@
     <t>Relevancia nosotros 2</t>
   </si>
   <si>
-    <t>Innovación nosotros 2</t>
-  </si>
-  <si>
-    <t>Espacios físicos aliados de la cultura nosotros 2</t>
-  </si>
-  <si>
     <t>Adaptabilidad nosotros 2</t>
   </si>
   <si>
@@ -1374,33 +1074,18 @@
     <t>Conciencia Sostenible nosotros 2</t>
   </si>
   <si>
-    <t>Servir con cercanía nosotros 2</t>
-  </si>
-  <si>
     <t>Superar metas nosotros 2</t>
   </si>
   <si>
-    <t>Conexión todos 1</t>
-  </si>
-  <si>
     <t>Equilibrio todos 1</t>
   </si>
   <si>
-    <t>Propósito todos 1</t>
-  </si>
-  <si>
     <t>Orgullo (eNps) todos 1</t>
   </si>
   <si>
     <t>Pedir ayuda todos 1</t>
   </si>
   <si>
-    <t>Contribución todos 1</t>
-  </si>
-  <si>
-    <t>Retroalimentación todos 1</t>
-  </si>
-  <si>
     <t>Reconocimiento todos 1</t>
   </si>
   <si>
@@ -1413,12 +1098,6 @@
     <t>Rituales todos 1</t>
   </si>
   <si>
-    <t>Comunicación todos 1</t>
-  </si>
-  <si>
-    <t>Contribución individual a la cultura todos 1</t>
-  </si>
-  <si>
     <t>Conversaciones todos 1</t>
   </si>
   <si>
@@ -1428,12 +1107,6 @@
     <t>Relevancia todos 1</t>
   </si>
   <si>
-    <t>Innovación todos 1</t>
-  </si>
-  <si>
-    <t>Espacios físicos aliados de la cultura todos 1</t>
-  </si>
-  <si>
     <t>Adaptabilidad todos 1</t>
   </si>
   <si>
@@ -1452,33 +1125,18 @@
     <t>Conciencia Sostenible todos 1</t>
   </si>
   <si>
-    <t>Servir con cercanía todos 1</t>
-  </si>
-  <si>
     <t>Superar metas todos 1</t>
   </si>
   <si>
-    <t>Conexión todos 2</t>
-  </si>
-  <si>
     <t>Equilibrio todos 2</t>
   </si>
   <si>
-    <t>Propósito todos 2</t>
-  </si>
-  <si>
     <t>Orgullo (eNps) todos 2</t>
   </si>
   <si>
     <t>Pedir ayuda todos 2</t>
   </si>
   <si>
-    <t>Contribución todos 2</t>
-  </si>
-  <si>
-    <t>Retroalimentación todos 2</t>
-  </si>
-  <si>
     <t>Reconocimiento todos 2</t>
   </si>
   <si>
@@ -1491,12 +1149,6 @@
     <t>Rituales todos 2</t>
   </si>
   <si>
-    <t>Comunicación todos 2</t>
-  </si>
-  <si>
-    <t>Contribución individual a la cultura todos 2</t>
-  </si>
-  <si>
     <t>Conversaciones todos 2</t>
   </si>
   <si>
@@ -1506,12 +1158,6 @@
     <t>Relevancia todos 2</t>
   </si>
   <si>
-    <t>Innovación todos 2</t>
-  </si>
-  <si>
-    <t>Espacios físicos aliados de la cultura todos 2</t>
-  </si>
-  <si>
     <t>Adaptabilidad todos 2</t>
   </si>
   <si>
@@ -1530,10 +1176,364 @@
     <t>Conciencia Sostenible todos 2</t>
   </si>
   <si>
-    <t>Servir con cercanía todos 2</t>
-  </si>
-  <si>
     <t>Superar metas todos 2</t>
+  </si>
+  <si>
+    <t>Conexion yo</t>
+  </si>
+  <si>
+    <t>Proposito yo</t>
+  </si>
+  <si>
+    <t>Contribucion yo</t>
+  </si>
+  <si>
+    <t>Retroalimentacion yo</t>
+  </si>
+  <si>
+    <t>Comunicacion yo</t>
+  </si>
+  <si>
+    <t>Contribucion individual a la cultura yo</t>
+  </si>
+  <si>
+    <t>Innovacion yo</t>
+  </si>
+  <si>
+    <t>Conexion nosotros 1</t>
+  </si>
+  <si>
+    <t>Tengo claras oportunidades de crecer dentro de mi equipo y de la organizacion</t>
+  </si>
+  <si>
+    <t>Proposito nosotros 1</t>
+  </si>
+  <si>
+    <t>Contribucion nosotros 1</t>
+  </si>
+  <si>
+    <t>Recibo retroalimentacion de mi jefe inmediato que me permite mejorar permanentemente</t>
+  </si>
+  <si>
+    <t>Retroalimentacion nosotros 1</t>
+  </si>
+  <si>
+    <t>Entiendo claramente mi rol y aporte a los resultados del equipo y de la organizacion</t>
+  </si>
+  <si>
+    <t>Comunicacion nosotros 1</t>
+  </si>
+  <si>
+    <t>Contribucion individual a la cultura nosotros 1</t>
+  </si>
+  <si>
+    <t>Tengo libertad para decidir como realizar mi trabajo</t>
+  </si>
+  <si>
+    <t>Innovacion nosotros 1</t>
+  </si>
+  <si>
+    <t>En nuestro equipo le damos mucho valor a la conciencia ecologica y se evidencia en las pequeñas decisiones cotidianas</t>
+  </si>
+  <si>
+    <t>Conexion nosotros 2</t>
+  </si>
+  <si>
+    <t>Tengo acceso a la informacion y recursos necesarios para realizar mi trabajo</t>
+  </si>
+  <si>
+    <t>Mi plan de carrera tiene futuro si permanezco en esta organizacion</t>
+  </si>
+  <si>
+    <t>Proposito nosotros 2</t>
+  </si>
+  <si>
+    <t>Mi relacion con mi jefe inmediato se basa en el respeto y la claridad</t>
+  </si>
+  <si>
+    <t>En el equipo cada uno sabe su tarea y es fundamental favorecer su concentracion para que la logre</t>
+  </si>
+  <si>
+    <t>Contribucion nosotros 2</t>
+  </si>
+  <si>
+    <t>Retroalimentacion nosotros 2</t>
+  </si>
+  <si>
+    <t>La comunicacion del equipo nos acerca como personas y facilita nuestros resultados</t>
+  </si>
+  <si>
+    <t>Comunicacion nosotros 2</t>
+  </si>
+  <si>
+    <t>Contribucion individual a la cultura nosotros 2</t>
+  </si>
+  <si>
+    <t>Innovacion nosotros 2</t>
+  </si>
+  <si>
+    <t>Conexion todos 1</t>
+  </si>
+  <si>
+    <t>La organizacion propicia un sano equilibrio vida/trabajo</t>
+  </si>
+  <si>
+    <t>El proposito de la organizacion me impulsa y saca lo mejor de mi</t>
+  </si>
+  <si>
+    <t>Proposito todos 1</t>
+  </si>
+  <si>
+    <t>Me siento orgulloso de ser parte del equipo humano de esta organizacion</t>
+  </si>
+  <si>
+    <t>En la organizacion las personas pedimos ayuda, la ofrecemos y la recibimos de parte de otros compañeros</t>
+  </si>
+  <si>
+    <t>En la organizacion todos contribuimos de manera destacada</t>
+  </si>
+  <si>
+    <t>Contribucion todos 1</t>
+  </si>
+  <si>
+    <t>Retroalimentacion todos 1</t>
+  </si>
+  <si>
+    <t>Mis resultados son reconocidos y valorados por la organizacion</t>
+  </si>
+  <si>
+    <t>En la organizacion celebramos los logros y aprendizajes</t>
+  </si>
+  <si>
+    <t>Somos una organizacion con buena comunicacion: escuchamos y somos escuchados y sabemos lo que pasa</t>
+  </si>
+  <si>
+    <t>Comunicacion todos 1</t>
+  </si>
+  <si>
+    <t>Las personas que trabajan en la organizacion imprimen sus propias cualidades en la cultura y la enriquecen</t>
+  </si>
+  <si>
+    <t>Contribucion individual a la cultura todos 1</t>
+  </si>
+  <si>
+    <t>En esta organizacion los espacios para conversar y escuchar son frecuentes y valorados</t>
+  </si>
+  <si>
+    <t>Innovacion todos 1</t>
+  </si>
+  <si>
+    <t>Los espacios de esta organizacion son excepcionales</t>
+  </si>
+  <si>
+    <t>La organizacion incorpora cambios con agilidad y capacidad de adaptacion</t>
+  </si>
+  <si>
+    <t>Nuestra organizacion se destaca por su contribucion a la sociedad</t>
+  </si>
+  <si>
+    <t>En esta organizacion se premia la proactividad y quienes se destacan suelen ser promovidos a nuevos retos</t>
+  </si>
+  <si>
+    <t>La organizacion trabaja en red y colabora con muchas otras organizaciones y personas. Esto nos enriquece a todos</t>
+  </si>
+  <si>
+    <t>En la organizacion se siente el colegaje y amistad tanto cuando cometemos errores como cuando obtenemos buenos resultados</t>
+  </si>
+  <si>
+    <t>La organizacion se destaca por obtener resultados excepcionales en todo lo que hace.</t>
+  </si>
+  <si>
+    <t>Me inspira la mision y proposito de la organizacion</t>
+  </si>
+  <si>
+    <t>Conexion todos 2</t>
+  </si>
+  <si>
+    <t>Los planes y proyectos nuevos de la organizacion se acompasan y conectan con el ritmo del equipo y sus planes previamente trazados</t>
+  </si>
+  <si>
+    <t>Proposito todos 2</t>
+  </si>
+  <si>
+    <t>Pedir ayuda es poco habitual en nuestra organizacion</t>
+  </si>
+  <si>
+    <t>En la organizacion tengo la oportunidad de mejorar mis habilidades</t>
+  </si>
+  <si>
+    <t>Contribucion todos 2</t>
+  </si>
+  <si>
+    <t>Retroalimentacion todos 2</t>
+  </si>
+  <si>
+    <t>La imagen que se percibe de la organizacion se corresponde con lo que yo vivo como colaborador</t>
+  </si>
+  <si>
+    <t>Tenemos serios problemas de comunicacion: no tenemos espacios para escucharnos y no siempre nos enteramos de lo que pasa</t>
+  </si>
+  <si>
+    <t>Comunicacion todos 2</t>
+  </si>
+  <si>
+    <t>Contribucion individual a la cultura todos 2</t>
+  </si>
+  <si>
+    <t>Me siento comodo en esta cultura y entorno organizacional</t>
+  </si>
+  <si>
+    <t>Innovacion todos 2</t>
+  </si>
+  <si>
+    <t>Los espacios de la organizacion son confortable y me aporta lo que necesito para estar bien</t>
+  </si>
+  <si>
+    <t>La organizacion se mueve despacio. Prefiere no tomar riesgos y cuida mucho su prestigio</t>
+  </si>
+  <si>
+    <t>Con frecuencia las decisiones de la organizacion ponen en riesgo su continuidad en el futuro</t>
+  </si>
+  <si>
+    <t>La organizacion suele ayudar a las causas sociales y situaciones de crisis que se presentan</t>
+  </si>
+  <si>
+    <t>La organizacion es considerada una organizacion influyente y con buenas conexiones</t>
+  </si>
+  <si>
+    <t>Tenemos mucho trabajo por delante para ganar conciencia ecologica en la organizacion</t>
+  </si>
+  <si>
+    <t>En la organizacion cooperamos cuando las personas cometen errores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con cual de las siguientes afirmaciones te identificas mas? </t>
+  </si>
+  <si>
+    <t>La dinamica de mi equipo de trabajo me permite experimentar un sano equilibrio entre la vida laboral y la vida personal</t>
+  </si>
+  <si>
+    <t>Estoy involucrado en el seguimiento de innovaciones y nuevos proyectos del area</t>
+  </si>
+  <si>
+    <t>Considero que mis pares estan abiertos a recibir opiniones diferentes a las suyas</t>
+  </si>
+  <si>
+    <t>Todos somos responsables de monitorear los riesgos del area</t>
+  </si>
+  <si>
+    <t>Los procesos y procedimientos estan muy claros y es indispensable seguirlos al pie de la letra</t>
+  </si>
+  <si>
+    <t>El proceso de nuestra area no suele tener muchas innovaciones</t>
+  </si>
+  <si>
+    <t>Se que hace cada persona de mi equipo. Les puedo ayudar y puedo contar con mis pares cuando necesito ayuda</t>
+  </si>
+  <si>
+    <t>Espacios fisicos aliados de la cultura yo</t>
+  </si>
+  <si>
+    <t>Servir con cercania yo</t>
+  </si>
+  <si>
+    <t>En nuestro equipo todos aportamos y el lider nos acompaña y direcciona para lograr resultados superiores a los esperados</t>
+  </si>
+  <si>
+    <t>Con mi equipo inmediato me siento en un entorno saludable fisica y emocionalmente</t>
+  </si>
+  <si>
+    <t>Espacios fisicos aliados de la cultura nosotros 1</t>
+  </si>
+  <si>
+    <t>Mi jefe es justo, claro y profesional para tomar decisiones. Confio en su criterio</t>
+  </si>
+  <si>
+    <t>Siento el respaldo de mi lider, incluso cuando cometo errores</t>
+  </si>
+  <si>
+    <t>Servir con cercania nosotros 1</t>
+  </si>
+  <si>
+    <t>Mi lider es claro con las metas y despliega incentivos claros para motivar resultados mas alla de lo esperado</t>
+  </si>
+  <si>
+    <t>El lider propicia espacios de encuentro y compartir como equipo</t>
+  </si>
+  <si>
+    <t>Yo me aseguro de no ser un problema para los demas. Otros deberian hacer lo mismo</t>
+  </si>
+  <si>
+    <t>Espacios fisicos aliados de la cultura nosotros 2</t>
+  </si>
+  <si>
+    <t>El lider es claro y asigna las tareas a cada persona para lograr los objetivos del equipo</t>
+  </si>
+  <si>
+    <t>Servir con cercania nosotros 2</t>
+  </si>
+  <si>
+    <t>Espacios fisicos aliados de la cultura todos 1</t>
+  </si>
+  <si>
+    <t>Servir con cercania todos 1</t>
+  </si>
+  <si>
+    <t>Mi familia y amigos se sienten orgullosos de que yo trabaje aqui</t>
+  </si>
+  <si>
+    <t>Trabajar aqui me hace sentir bienestar. Me siento protegido y tranquilo</t>
+  </si>
+  <si>
+    <t>Espacios fisicos aliados de la cultura todos 2</t>
+  </si>
+  <si>
+    <t>Servir con cercania todos 2</t>
+  </si>
+  <si>
+    <t>Los valores que promueve la organizacion corresponden con los mios</t>
+  </si>
+  <si>
+    <t>Retroalimentar el trabajo propio y de los demas para aprender juntos es un habito de nuestra organizacion</t>
+  </si>
+  <si>
+    <t>Me gusta la personalidad de esta organizacion. Proyecta confianza y es afin a mi estilo de vida</t>
+  </si>
+  <si>
+    <t>Confio en los lideres de la organizacion</t>
+  </si>
+  <si>
+    <t>En la organizacion se respira un ambiente de tranquilidad y armonia</t>
+  </si>
+  <si>
+    <t>Uno de los atributos mas visibles de nuestra organizacion es la innovacion</t>
+  </si>
+  <si>
+    <t>La organizacion se destaca por sus practicas medioambientales y de sostenibilidad</t>
+  </si>
+  <si>
+    <t>Las maneras actuales de priorizar y actuar en la organizacion nos estan acercando al proposito y plan estrategico trazado</t>
+  </si>
+  <si>
+    <t>Los espacios formales de retroalimentacion son pocos y podrian ser mas productivos</t>
+  </si>
+  <si>
+    <t>Todos los que van llegando nuevos a la organizacion se adaptan a la cultura y se ajustan a las maneras en que aqui se hacen las cosas</t>
+  </si>
+  <si>
+    <t>Cada equipo tiene sus propios retos y resultados. En esta organizacion todos somos muy distintos y poco interactuamos entre areas distintas</t>
+  </si>
+  <si>
+    <t>La organizacion es principalmente conservadora y clasica</t>
+  </si>
+  <si>
+    <t>Cada persona de la organizacion esta comprometida con los resultados</t>
+  </si>
+  <si>
+    <t>La organizacion se destaca ante la sociedad en los campos mas significativos de su trabajo</t>
+  </si>
+  <si>
+    <t>Las decisiones que ha tomado la organizacion en el ultimo año nos llevaran mas lejos y estan alineadas a los objetivos</t>
   </si>
 </sst>
 </file>
@@ -1969,7 +1969,7 @@
   <dimension ref="A1:E131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1980,2229 +1980,2229 @@
   <sheetData>
     <row r="1" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>107</v>
+        <v>33</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>106</v>
+        <v>32</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>105</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>238</v>
+        <v>164</v>
       </c>
       <c r="E1" t="s">
-        <v>369</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>108</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>370</v>
+        <v>381</v>
       </c>
       <c r="E2" t="s">
-        <v>239</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>109</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>371</v>
+        <v>296</v>
       </c>
       <c r="E3" t="s">
-        <v>240</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="E4" t="s">
-        <v>241</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>111</v>
+        <v>37</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>373</v>
+        <v>297</v>
       </c>
       <c r="E5" t="s">
-        <v>242</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>112</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C6" s="1">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>374</v>
+        <v>298</v>
       </c>
       <c r="E6" t="s">
-        <v>243</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>113</v>
+        <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>375</v>
+        <v>383</v>
       </c>
       <c r="E7" t="s">
-        <v>244</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>114</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C8" s="1">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>376</v>
+        <v>384</v>
       </c>
       <c r="E8" t="s">
-        <v>245</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>115</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>377</v>
+        <v>299</v>
       </c>
       <c r="E9" t="s">
-        <v>246</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>116</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C10" s="1">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>378</v>
+        <v>300</v>
       </c>
       <c r="E10" t="s">
-        <v>247</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>117</v>
+        <v>43</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C11" s="1">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>379</v>
+        <v>301</v>
       </c>
       <c r="E11" t="s">
-        <v>248</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>118</v>
+        <v>44</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C12" s="1">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>380</v>
+        <v>302</v>
       </c>
       <c r="E12" t="s">
-        <v>249</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>119</v>
+        <v>45</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="E13" t="s">
-        <v>250</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>120</v>
+        <v>46</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="E14" t="s">
-        <v>251</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>121</v>
+        <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>383</v>
+        <v>303</v>
       </c>
       <c r="E15" t="s">
-        <v>252</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>122</v>
+        <v>48</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>384</v>
+        <v>304</v>
       </c>
       <c r="E16" t="s">
-        <v>253</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>123</v>
+        <v>49</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>385</v>
+        <v>305</v>
       </c>
       <c r="E17" t="s">
-        <v>254</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>124</v>
+        <v>50</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="E18" t="s">
-        <v>255</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>125</v>
+        <v>51</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>387</v>
+        <v>465</v>
       </c>
       <c r="E19" t="s">
-        <v>256</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>126</v>
+        <v>52</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>388</v>
+        <v>306</v>
       </c>
       <c r="E20" t="s">
-        <v>257</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>127</v>
+        <v>53</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C21" s="1">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>389</v>
+        <v>307</v>
       </c>
       <c r="E21" t="s">
-        <v>258</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>128</v>
+        <v>54</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>390</v>
+        <v>308</v>
       </c>
       <c r="E22" t="s">
-        <v>259</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>129</v>
+        <v>55</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>391</v>
+        <v>309</v>
       </c>
       <c r="E23" t="s">
-        <v>260</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>130</v>
+        <v>56</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C24" s="1">
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>392</v>
+        <v>310</v>
       </c>
       <c r="E24" t="s">
-        <v>261</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>131</v>
+        <v>57</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C25" s="1">
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>393</v>
+        <v>311</v>
       </c>
       <c r="E25" t="s">
-        <v>262</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>132</v>
+        <v>58</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C26" s="1">
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>394</v>
+        <v>466</v>
       </c>
       <c r="E26" t="s">
-        <v>263</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>133</v>
+        <v>59</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>104</v>
+        <v>457</v>
       </c>
       <c r="C27" s="1">
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>395</v>
+        <v>312</v>
       </c>
       <c r="E27" t="s">
-        <v>264</v>
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>134</v>
+        <v>60</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>103</v>
+        <v>30</v>
       </c>
       <c r="C28" s="1">
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="E28" t="s">
-        <v>265</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>135</v>
+        <v>61</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>102</v>
+        <v>458</v>
       </c>
       <c r="C29" s="1">
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>397</v>
+        <v>313</v>
       </c>
       <c r="E29" t="s">
-        <v>266</v>
+        <v>192</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>136</v>
+        <v>62</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>101</v>
+        <v>389</v>
       </c>
       <c r="C30" s="1">
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="E30" t="s">
-        <v>267</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>100</v>
+        <v>29</v>
       </c>
       <c r="C31" s="1">
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>399</v>
+        <v>314</v>
       </c>
       <c r="E31" t="s">
-        <v>268</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>138</v>
+        <v>64</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>99</v>
+        <v>28</v>
       </c>
       <c r="C32" s="1">
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>400</v>
+        <v>315</v>
       </c>
       <c r="E32" t="s">
-        <v>269</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>139</v>
+        <v>65</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>98</v>
+        <v>27</v>
       </c>
       <c r="C33" s="1">
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="E33" t="s">
-        <v>270</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>140</v>
+        <v>66</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>97</v>
+        <v>392</v>
       </c>
       <c r="C34" s="1">
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="E34" t="s">
-        <v>271</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>141</v>
+        <v>67</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>96</v>
+        <v>26</v>
       </c>
       <c r="C35" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D35" t="s">
-        <v>403</v>
+        <v>316</v>
       </c>
       <c r="E35" t="s">
-        <v>272</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>142</v>
+        <v>68</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>95</v>
+        <v>394</v>
       </c>
       <c r="C36" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D36" t="s">
-        <v>404</v>
+        <v>317</v>
       </c>
       <c r="E36" t="s">
-        <v>273</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>143</v>
+        <v>69</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>94</v>
+        <v>467</v>
       </c>
       <c r="C37" s="1">
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>405</v>
+        <v>318</v>
       </c>
       <c r="E37" t="s">
-        <v>274</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>144</v>
+        <v>70</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>93</v>
+        <v>25</v>
       </c>
       <c r="C38" s="1">
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>406</v>
+        <v>319</v>
       </c>
       <c r="E38" t="s">
-        <v>275</v>
+        <v>201</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>145</v>
+        <v>71</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>92</v>
+        <v>24</v>
       </c>
       <c r="C39" s="1">
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="E39" t="s">
-        <v>276</v>
+        <v>202</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>146</v>
+        <v>72</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="C40" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D40" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="E40" t="s">
-        <v>277</v>
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>147</v>
+        <v>73</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>90</v>
+        <v>22</v>
       </c>
       <c r="C41" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D41" t="s">
-        <v>409</v>
+        <v>320</v>
       </c>
       <c r="E41" t="s">
-        <v>278</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>148</v>
+        <v>74</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>89</v>
+        <v>468</v>
       </c>
       <c r="C42" s="1">
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>410</v>
+        <v>321</v>
       </c>
       <c r="E42" t="s">
-        <v>279</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>149</v>
+        <v>75</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>88</v>
+        <v>397</v>
       </c>
       <c r="C43" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D43" t="s">
-        <v>411</v>
+        <v>322</v>
       </c>
       <c r="E43" t="s">
-        <v>280</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>150</v>
+        <v>76</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>87</v>
+        <v>459</v>
       </c>
       <c r="C44" s="1">
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="E44" t="s">
-        <v>281</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>151</v>
+        <v>77</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="C45" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D45" t="s">
-        <v>413</v>
+        <v>469</v>
       </c>
       <c r="E45" t="s">
-        <v>282</v>
+        <v>208</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>152</v>
+        <v>78</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="C46" s="1">
         <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>414</v>
+        <v>323</v>
       </c>
       <c r="E46" t="s">
-        <v>283</v>
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>153</v>
+        <v>79</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>84</v>
+        <v>470</v>
       </c>
       <c r="C47" s="1">
         <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>415</v>
+        <v>324</v>
       </c>
       <c r="E47" t="s">
-        <v>284</v>
+        <v>210</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>154</v>
+        <v>80</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="C48" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D48" t="s">
-        <v>416</v>
+        <v>325</v>
       </c>
       <c r="E48" t="s">
-        <v>285</v>
+        <v>211</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>155</v>
+        <v>81</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="C49" s="1">
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>417</v>
+        <v>326</v>
       </c>
       <c r="E49" t="s">
-        <v>286</v>
+        <v>212</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>156</v>
+        <v>82</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="C50" s="1">
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>418</v>
+        <v>327</v>
       </c>
       <c r="E50" t="s">
-        <v>287</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>157</v>
+        <v>83</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>80</v>
+        <v>399</v>
       </c>
       <c r="C51" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D51" t="s">
-        <v>419</v>
+        <v>328</v>
       </c>
       <c r="E51" t="s">
-        <v>288</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>158</v>
+        <v>84</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>79</v>
+        <v>471</v>
       </c>
       <c r="C52" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D52" t="s">
-        <v>420</v>
+        <v>472</v>
       </c>
       <c r="E52" t="s">
-        <v>289</v>
+        <v>215</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>159</v>
+        <v>85</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>78</v>
+        <v>473</v>
       </c>
       <c r="C53" s="1">
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>421</v>
+        <v>329</v>
       </c>
       <c r="E53" t="s">
-        <v>290</v>
+        <v>216</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>160</v>
+        <v>86</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="C54" s="1">
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>422</v>
+        <v>400</v>
       </c>
       <c r="E54" t="s">
-        <v>291</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>161</v>
+        <v>87</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>76</v>
+        <v>401</v>
       </c>
       <c r="C55" s="1">
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>423</v>
+        <v>330</v>
       </c>
       <c r="E55" t="s">
-        <v>292</v>
+        <v>218</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>162</v>
+        <v>88</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>75</v>
+        <v>402</v>
       </c>
       <c r="C56" s="1">
         <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>424</v>
+        <v>403</v>
       </c>
       <c r="E56" t="s">
-        <v>293</v>
+        <v>219</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>163</v>
+        <v>89</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>74</v>
+        <v>404</v>
       </c>
       <c r="C57" s="1">
         <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>425</v>
+        <v>331</v>
       </c>
       <c r="E57" t="s">
-        <v>294</v>
+        <v>220</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>164</v>
+        <v>90</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>73</v>
+        <v>405</v>
       </c>
       <c r="C58" s="1">
         <v>0</v>
       </c>
       <c r="D58" t="s">
-        <v>426</v>
+        <v>332</v>
       </c>
       <c r="E58" t="s">
-        <v>295</v>
+        <v>221</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>165</v>
+        <v>91</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>72</v>
+        <v>460</v>
       </c>
       <c r="C59" s="1">
         <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>427</v>
+        <v>406</v>
       </c>
       <c r="E59" t="s">
-        <v>296</v>
+        <v>222</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>166</v>
+        <v>92</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>71</v>
+        <v>461</v>
       </c>
       <c r="C60" s="1">
         <v>0</v>
       </c>
       <c r="D60" t="s">
-        <v>428</v>
+        <v>407</v>
       </c>
       <c r="E60" t="s">
-        <v>297</v>
+        <v>223</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>167</v>
+        <v>93</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="C61" s="1">
         <v>0</v>
       </c>
       <c r="D61" t="s">
-        <v>429</v>
+        <v>333</v>
       </c>
       <c r="E61" t="s">
-        <v>298</v>
+        <v>224</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>168</v>
+        <v>94</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="C62" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D62" t="s">
-        <v>430</v>
+        <v>334</v>
       </c>
       <c r="E62" t="s">
-        <v>299</v>
+        <v>225</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>169</v>
+        <v>95</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="C63" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D63" t="s">
-        <v>431</v>
+        <v>335</v>
       </c>
       <c r="E63" t="s">
-        <v>300</v>
+        <v>226</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>170</v>
+        <v>96</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>67</v>
+        <v>474</v>
       </c>
       <c r="C64" s="1">
         <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>432</v>
+        <v>336</v>
       </c>
       <c r="E64" t="s">
-        <v>301</v>
+        <v>227</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>171</v>
+        <v>97</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>66</v>
+        <v>408</v>
       </c>
       <c r="C65" s="1">
         <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>433</v>
+        <v>409</v>
       </c>
       <c r="E65" t="s">
-        <v>302</v>
+        <v>228</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>172</v>
+        <v>98</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="C66" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D66" t="s">
-        <v>434</v>
+        <v>410</v>
       </c>
       <c r="E66" t="s">
-        <v>303</v>
+        <v>229</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>173</v>
+        <v>99</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="C67" s="1">
         <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>435</v>
+        <v>337</v>
       </c>
       <c r="E67" t="s">
-        <v>304</v>
+        <v>230</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>174</v>
+        <v>100</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>63</v>
+        <v>475</v>
       </c>
       <c r="C68" s="1">
         <v>0</v>
       </c>
       <c r="D68" t="s">
-        <v>436</v>
+        <v>338</v>
       </c>
       <c r="E68" t="s">
-        <v>305</v>
+        <v>231</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>175</v>
+        <v>101</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>62</v>
+        <v>462</v>
       </c>
       <c r="C69" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D69" t="s">
-        <v>437</v>
+        <v>339</v>
       </c>
       <c r="E69" t="s">
-        <v>306</v>
+        <v>232</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>176</v>
+        <v>102</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>61</v>
+        <v>463</v>
       </c>
       <c r="C70" s="1">
         <v>1</v>
       </c>
       <c r="D70" t="s">
-        <v>438</v>
+        <v>411</v>
       </c>
       <c r="E70" t="s">
-        <v>307</v>
+        <v>233</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>177</v>
+        <v>103</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C71" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D71" t="s">
-        <v>439</v>
+        <v>476</v>
       </c>
       <c r="E71" t="s">
-        <v>308</v>
+        <v>234</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>178</v>
+        <v>104</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="C72" s="1">
         <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>440</v>
+        <v>340</v>
       </c>
       <c r="E72" t="s">
-        <v>309</v>
+        <v>235</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>179</v>
+        <v>105</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>58</v>
+        <v>464</v>
       </c>
       <c r="C73" s="1">
         <v>0</v>
       </c>
       <c r="D73" t="s">
-        <v>441</v>
+        <v>341</v>
       </c>
       <c r="E73" t="s">
-        <v>310</v>
+        <v>236</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>180</v>
+        <v>106</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="C74" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D74" t="s">
-        <v>442</v>
+        <v>342</v>
       </c>
       <c r="E74" t="s">
-        <v>311</v>
+        <v>237</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>181</v>
+        <v>107</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>56</v>
+        <v>477</v>
       </c>
       <c r="C75" s="1">
         <v>0</v>
       </c>
       <c r="D75" t="s">
-        <v>443</v>
+        <v>343</v>
       </c>
       <c r="E75" t="s">
-        <v>312</v>
+        <v>238</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>182</v>
+        <v>108</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="C76" s="1">
         <v>0</v>
       </c>
       <c r="D76" t="s">
-        <v>444</v>
+        <v>344</v>
       </c>
       <c r="E76" t="s">
-        <v>313</v>
+        <v>239</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>183</v>
+        <v>109</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="C77" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D77" t="s">
-        <v>445</v>
+        <v>345</v>
       </c>
       <c r="E77" t="s">
-        <v>314</v>
+        <v>240</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>184</v>
+        <v>110</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C78" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D78" t="s">
-        <v>446</v>
+        <v>478</v>
       </c>
       <c r="E78" t="s">
-        <v>315</v>
+        <v>241</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>185</v>
+        <v>111</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="C79" s="1">
         <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>447</v>
+        <v>346</v>
       </c>
       <c r="E79" t="s">
-        <v>316</v>
+        <v>242</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>186</v>
+        <v>112</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>51</v>
+        <v>485</v>
       </c>
       <c r="C80" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D80" t="s">
-        <v>448</v>
+        <v>412</v>
       </c>
       <c r="E80" t="s">
-        <v>317</v>
+        <v>243</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>187</v>
+        <v>113</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>50</v>
+        <v>413</v>
       </c>
       <c r="C81" s="1">
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>449</v>
+        <v>347</v>
       </c>
       <c r="E81" t="s">
-        <v>318</v>
+        <v>244</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>188</v>
+        <v>114</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>49</v>
+        <v>414</v>
       </c>
       <c r="C82" s="1">
         <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>450</v>
+        <v>415</v>
       </c>
       <c r="E82" t="s">
-        <v>319</v>
+        <v>245</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>189</v>
+        <v>115</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>48</v>
+        <v>416</v>
       </c>
       <c r="C83" s="1">
         <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>451</v>
+        <v>348</v>
       </c>
       <c r="E83" t="s">
-        <v>320</v>
+        <v>246</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>190</v>
+        <v>116</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>47</v>
+        <v>417</v>
       </c>
       <c r="C84" s="1">
         <v>0</v>
       </c>
       <c r="D84" t="s">
-        <v>452</v>
+        <v>349</v>
       </c>
       <c r="E84" t="s">
-        <v>321</v>
+        <v>247</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>191</v>
+        <v>117</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>46</v>
+        <v>418</v>
       </c>
       <c r="C85" s="1">
         <v>0</v>
       </c>
       <c r="D85" t="s">
-        <v>453</v>
+        <v>419</v>
       </c>
       <c r="E85" t="s">
-        <v>322</v>
+        <v>248</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>192</v>
+        <v>118</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>45</v>
+        <v>486</v>
       </c>
       <c r="C86" s="1">
         <v>0</v>
       </c>
       <c r="D86" t="s">
-        <v>454</v>
+        <v>420</v>
       </c>
       <c r="E86" t="s">
-        <v>323</v>
+        <v>249</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>193</v>
+        <v>119</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>44</v>
+        <v>421</v>
       </c>
       <c r="C87" s="1">
         <v>0</v>
       </c>
       <c r="D87" t="s">
-        <v>455</v>
+        <v>350</v>
       </c>
       <c r="E87" t="s">
-        <v>324</v>
+        <v>250</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>194</v>
+        <v>120</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>43</v>
+        <v>487</v>
       </c>
       <c r="C88" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D88" t="s">
-        <v>456</v>
+        <v>351</v>
       </c>
       <c r="E88" t="s">
-        <v>325</v>
+        <v>251</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>195</v>
+        <v>121</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>42</v>
+        <v>488</v>
       </c>
       <c r="C89" s="1">
         <v>0</v>
       </c>
       <c r="D89" t="s">
-        <v>457</v>
+        <v>352</v>
       </c>
       <c r="E89" t="s">
-        <v>326</v>
+        <v>252</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>196</v>
+        <v>122</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>41</v>
+        <v>422</v>
       </c>
       <c r="C90" s="1">
         <v>0</v>
       </c>
       <c r="D90" t="s">
-        <v>458</v>
+        <v>353</v>
       </c>
       <c r="E90" t="s">
-        <v>327</v>
+        <v>253</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>197</v>
+        <v>123</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>40</v>
+        <v>423</v>
       </c>
       <c r="C91" s="1">
         <v>0</v>
       </c>
       <c r="D91" t="s">
-        <v>459</v>
+        <v>424</v>
       </c>
       <c r="E91" t="s">
-        <v>328</v>
+        <v>254</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>198</v>
+        <v>124</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>39</v>
+        <v>425</v>
       </c>
       <c r="C92" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D92" t="s">
-        <v>460</v>
+        <v>426</v>
       </c>
       <c r="E92" t="s">
-        <v>329</v>
+        <v>255</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>199</v>
+        <v>125</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>38</v>
+        <v>427</v>
       </c>
       <c r="C93" s="1">
         <v>0</v>
       </c>
       <c r="D93" t="s">
-        <v>461</v>
+        <v>354</v>
       </c>
       <c r="E93" t="s">
-        <v>330</v>
+        <v>256</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>200</v>
+        <v>126</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>37</v>
+        <v>489</v>
       </c>
       <c r="C94" s="1">
         <v>0</v>
       </c>
       <c r="D94" t="s">
-        <v>462</v>
+        <v>355</v>
       </c>
       <c r="E94" t="s">
-        <v>331</v>
+        <v>257</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>201</v>
+        <v>127</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="C95" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D95" t="s">
-        <v>463</v>
+        <v>356</v>
       </c>
       <c r="E95" t="s">
-        <v>332</v>
+        <v>258</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>202</v>
+        <v>128</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>35</v>
+        <v>490</v>
       </c>
       <c r="C96" s="1">
         <v>0</v>
       </c>
       <c r="D96" t="s">
-        <v>464</v>
+        <v>428</v>
       </c>
       <c r="E96" t="s">
-        <v>333</v>
+        <v>259</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>203</v>
+        <v>129</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>34</v>
+        <v>429</v>
       </c>
       <c r="C97" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D97" t="s">
-        <v>465</v>
+        <v>479</v>
       </c>
       <c r="E97" t="s">
-        <v>334</v>
+        <v>260</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>204</v>
+        <v>130</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>33</v>
+        <v>430</v>
       </c>
       <c r="C98" s="1">
         <v>0</v>
       </c>
       <c r="D98" t="s">
-        <v>466</v>
+        <v>357</v>
       </c>
       <c r="E98" t="s">
-        <v>335</v>
+        <v>261</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>205</v>
+        <v>131</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>32</v>
+        <v>499</v>
       </c>
       <c r="C99" s="1">
         <v>0</v>
       </c>
       <c r="D99" t="s">
-        <v>467</v>
+        <v>358</v>
       </c>
       <c r="E99" t="s">
-        <v>336</v>
+        <v>262</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>206</v>
+        <v>132</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>31</v>
+        <v>431</v>
       </c>
       <c r="C100" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D100" t="s">
-        <v>468</v>
+        <v>359</v>
       </c>
       <c r="E100" t="s">
-        <v>337</v>
+        <v>263</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>207</v>
+        <v>133</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>30</v>
+        <v>432</v>
       </c>
       <c r="C101" s="1">
         <v>0</v>
       </c>
       <c r="D101" t="s">
-        <v>469</v>
+        <v>360</v>
       </c>
       <c r="E101" t="s">
-        <v>338</v>
+        <v>264</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>208</v>
+        <v>134</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>29</v>
+        <v>433</v>
       </c>
       <c r="C102" s="1">
         <v>0</v>
       </c>
       <c r="D102" t="s">
-        <v>470</v>
+        <v>361</v>
       </c>
       <c r="E102" t="s">
-        <v>339</v>
+        <v>265</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>209</v>
+        <v>135</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>28</v>
+        <v>491</v>
       </c>
       <c r="C103" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D103" t="s">
-        <v>471</v>
+        <v>362</v>
       </c>
       <c r="E103" t="s">
-        <v>340</v>
+        <v>266</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>210</v>
+        <v>136</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>27</v>
+        <v>434</v>
       </c>
       <c r="C104" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D104" t="s">
-        <v>472</v>
+        <v>480</v>
       </c>
       <c r="E104" t="s">
-        <v>341</v>
+        <v>267</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>211</v>
+        <v>137</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>26</v>
+        <v>435</v>
       </c>
       <c r="C105" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D105" t="s">
-        <v>473</v>
+        <v>363</v>
       </c>
       <c r="E105" t="s">
-        <v>342</v>
+        <v>268</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>212</v>
+        <v>138</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>25</v>
+        <v>436</v>
       </c>
       <c r="C106" s="1">
         <v>0</v>
       </c>
       <c r="D106" t="s">
-        <v>474</v>
+        <v>437</v>
       </c>
       <c r="E106" t="s">
-        <v>343</v>
+        <v>269</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>213</v>
+        <v>139</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>24</v>
+        <v>438</v>
       </c>
       <c r="C107" s="1">
         <v>0</v>
       </c>
       <c r="D107" t="s">
-        <v>475</v>
+        <v>364</v>
       </c>
       <c r="E107" t="s">
-        <v>344</v>
+        <v>270</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>214</v>
+        <v>140</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>23</v>
+        <v>492</v>
       </c>
       <c r="C108" s="1">
         <v>0</v>
       </c>
       <c r="D108" t="s">
-        <v>476</v>
+        <v>439</v>
       </c>
       <c r="E108" t="s">
-        <v>345</v>
+        <v>271</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>215</v>
+        <v>141</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>22</v>
+        <v>481</v>
       </c>
       <c r="C109" s="1">
         <v>0</v>
       </c>
       <c r="D109" t="s">
-        <v>477</v>
+        <v>365</v>
       </c>
       <c r="E109" t="s">
-        <v>346</v>
+        <v>272</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>216</v>
+        <v>142</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>21</v>
+        <v>440</v>
       </c>
       <c r="C110" s="1">
         <v>1</v>
       </c>
       <c r="D110" t="s">
-        <v>478</v>
+        <v>366</v>
       </c>
       <c r="E110" t="s">
-        <v>347</v>
+        <v>273</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>217</v>
+        <v>143</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>20</v>
+        <v>441</v>
       </c>
       <c r="C111" s="1">
         <v>0</v>
       </c>
       <c r="D111" t="s">
-        <v>479</v>
+        <v>442</v>
       </c>
       <c r="E111" t="s">
-        <v>348</v>
+        <v>274</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>218</v>
+        <v>144</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>19</v>
+        <v>493</v>
       </c>
       <c r="C112" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D112" t="s">
-        <v>480</v>
+        <v>443</v>
       </c>
       <c r="E112" t="s">
-        <v>349</v>
+        <v>275</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>219</v>
+        <v>145</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C113" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D113" t="s">
-        <v>481</v>
+        <v>367</v>
       </c>
       <c r="E113" t="s">
-        <v>350</v>
+        <v>276</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>220</v>
+        <v>146</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>17</v>
+        <v>444</v>
       </c>
       <c r="C114" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D114" t="s">
-        <v>482</v>
+        <v>368</v>
       </c>
       <c r="E114" t="s">
-        <v>351</v>
+        <v>277</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>221</v>
+        <v>147</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C115" s="1">
         <v>0</v>
       </c>
       <c r="D115" t="s">
-        <v>483</v>
+        <v>369</v>
       </c>
       <c r="E115" t="s">
-        <v>352</v>
+        <v>278</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>222</v>
+        <v>148</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C116" s="1">
         <v>0</v>
       </c>
       <c r="D116" t="s">
-        <v>484</v>
+        <v>370</v>
       </c>
       <c r="E116" t="s">
-        <v>353</v>
+        <v>279</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>223</v>
+        <v>149</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>14</v>
+        <v>445</v>
       </c>
       <c r="C117" s="1">
         <v>1</v>
       </c>
       <c r="D117" t="s">
-        <v>485</v>
+        <v>446</v>
       </c>
       <c r="E117" t="s">
-        <v>354</v>
+        <v>280</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>224</v>
+        <v>150</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>13</v>
+        <v>494</v>
       </c>
       <c r="C118" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D118" t="s">
-        <v>486</v>
+        <v>447</v>
       </c>
       <c r="E118" t="s">
-        <v>355</v>
+        <v>281</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>225</v>
+        <v>151</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>12</v>
+        <v>495</v>
       </c>
       <c r="C119" s="1">
         <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>487</v>
+        <v>371</v>
       </c>
       <c r="E119" t="s">
-        <v>356</v>
+        <v>282</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>226</v>
+        <v>152</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>11</v>
+        <v>482</v>
       </c>
       <c r="C120" s="1">
         <v>0</v>
       </c>
       <c r="D120" t="s">
-        <v>488</v>
+        <v>372</v>
       </c>
       <c r="E120" t="s">
-        <v>357</v>
+        <v>283</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>227</v>
+        <v>153</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>10</v>
+        <v>448</v>
       </c>
       <c r="C121" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D121" t="s">
-        <v>489</v>
+        <v>373</v>
       </c>
       <c r="E121" t="s">
-        <v>358</v>
+        <v>284</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>228</v>
+        <v>154</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>9</v>
+        <v>496</v>
       </c>
       <c r="C122" s="1">
         <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>490</v>
+        <v>449</v>
       </c>
       <c r="E122" t="s">
-        <v>359</v>
+        <v>285</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>229</v>
+        <v>155</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>8</v>
+        <v>450</v>
       </c>
       <c r="C123" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D123" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="E123" t="s">
-        <v>360</v>
+        <v>286</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>230</v>
+        <v>156</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>7</v>
+        <v>451</v>
       </c>
       <c r="C124" s="1">
         <v>1</v>
       </c>
       <c r="D124" t="s">
-        <v>492</v>
+        <v>374</v>
       </c>
       <c r="E124" t="s">
-        <v>361</v>
+        <v>287</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>231</v>
+        <v>157</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>6</v>
+        <v>452</v>
       </c>
       <c r="C125" s="1">
         <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>493</v>
+        <v>375</v>
       </c>
       <c r="E125" t="s">
-        <v>362</v>
+        <v>288</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>232</v>
+        <v>158</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>5</v>
+        <v>453</v>
       </c>
       <c r="C126" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D126" t="s">
-        <v>494</v>
+        <v>376</v>
       </c>
       <c r="E126" t="s">
-        <v>363</v>
+        <v>289</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>233</v>
+        <v>159</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>4</v>
+        <v>497</v>
       </c>
       <c r="C127" s="1">
         <v>0</v>
       </c>
       <c r="D127" t="s">
-        <v>495</v>
+        <v>377</v>
       </c>
       <c r="E127" t="s">
-        <v>364</v>
+        <v>290</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>234</v>
+        <v>160</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>3</v>
+        <v>454</v>
       </c>
       <c r="C128" s="1">
         <v>0</v>
       </c>
       <c r="D128" t="s">
-        <v>496</v>
+        <v>378</v>
       </c>
       <c r="E128" t="s">
-        <v>365</v>
+        <v>291</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>235</v>
+        <v>161</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>2</v>
+        <v>455</v>
       </c>
       <c r="C129" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D129" t="s">
-        <v>497</v>
+        <v>379</v>
       </c>
       <c r="E129" t="s">
-        <v>366</v>
+        <v>292</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>236</v>
+        <v>162</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>1</v>
+        <v>456</v>
       </c>
       <c r="C130" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D130" t="s">
-        <v>498</v>
+        <v>484</v>
       </c>
       <c r="E130" t="s">
-        <v>367</v>
+        <v>293</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>237</v>
+        <v>163</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>0</v>
+        <v>498</v>
       </c>
       <c r="C131" s="1">
         <v>0</v>
       </c>
       <c r="D131" t="s">
-        <v>499</v>
+        <v>380</v>
       </c>
       <c r="E131" t="s">
-        <v>368</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizacion de scripts que genera las variables insumo y las correlaciones, creacion de la vista en tableu version 1
</commit_message>
<xml_diff>
--- a/misc/catalogos/catalogo_1.xlsx
+++ b/misc/catalogos/catalogo_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yeimunoz\Documents\caramelo\catalogos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berse\Documents\Caramelo escaso\caramelo\misc\catalogos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57E8FE6-3AC4-4D20-98BA-F29EFC909B54}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBE3735-315D-4C11-AAEB-718F4CE70658}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{855AF920-00D3-496D-A6BC-53AC25B09997}"/>
   </bookViews>
@@ -18,23 +18,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Catalogo_1!$A$1:$C$131</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="402">
   <si>
     <t>Las celebraciones de la empresa nos permiten integrarnos y pasar un tiempo juntos</t>
   </si>
@@ -924,366 +918,42 @@
     <t>id_pnt</t>
   </si>
   <si>
-    <t>Equilibrio yo</t>
-  </si>
-  <si>
-    <t>Orgullo (eNps) yo</t>
-  </si>
-  <si>
-    <t>Pedir ayuda yo</t>
-  </si>
-  <si>
-    <t>Reconocimiento yo</t>
-  </si>
-  <si>
-    <t>Claridad en ADN: personalidad de mi empresa yo</t>
-  </si>
-  <si>
-    <t>Liderazgo y trabajo en equipo yo</t>
-  </si>
-  <si>
-    <t>Rituales yo</t>
-  </si>
-  <si>
-    <t>Conversaciones yo</t>
-  </si>
-  <si>
-    <t>Entorno saludable yo</t>
-  </si>
-  <si>
-    <t>Relevancia yo</t>
-  </si>
-  <si>
-    <t>Adaptabilidad yo</t>
-  </si>
-  <si>
-    <t>Toma de decisiones yo</t>
-  </si>
-  <si>
-    <t>Impacto en la sociedad yo</t>
-  </si>
-  <si>
-    <t>Empoderamiento yo</t>
-  </si>
-  <si>
-    <t>Relaciones yo</t>
-  </si>
-  <si>
-    <t>Conciencia Sostenible yo</t>
-  </si>
-  <si>
-    <t>Superar metas yo</t>
-  </si>
-  <si>
-    <t>Equilibrio nosotros 1</t>
-  </si>
-  <si>
-    <t>Orgullo (eNps) nosotros 1</t>
-  </si>
-  <si>
-    <t>Pedir ayuda nosotros 1</t>
-  </si>
-  <si>
-    <t>Reconocimiento nosotros 1</t>
-  </si>
-  <si>
-    <t>Claridad en ADN: personalidad de mi empresa nosotros 1</t>
-  </si>
-  <si>
-    <t>Liderazgo y trabajo en equipo nosotros 1</t>
-  </si>
-  <si>
-    <t>Rituales nosotros 1</t>
-  </si>
-  <si>
-    <t>Conversaciones nosotros 1</t>
-  </si>
-  <si>
-    <t>Entorno saludable nosotros 1</t>
-  </si>
-  <si>
-    <t>Relevancia nosotros 1</t>
-  </si>
-  <si>
-    <t>Adaptabilidad nosotros 1</t>
-  </si>
-  <si>
-    <t>Toma de decisiones nosotros 1</t>
-  </si>
-  <si>
-    <t>Impacto en la sociedad nosotros 1</t>
-  </si>
-  <si>
-    <t>Empoderamiento nosotros 1</t>
-  </si>
-  <si>
-    <t>Relaciones nosotros 1</t>
-  </si>
-  <si>
-    <t>Conciencia Sostenible nosotros 1</t>
-  </si>
-  <si>
-    <t>Superar metas nosotros 1</t>
-  </si>
-  <si>
-    <t>Equilibrio nosotros 2</t>
-  </si>
-  <si>
-    <t>Orgullo (eNps) nosotros 2</t>
-  </si>
-  <si>
-    <t>Pedir ayuda nosotros 2</t>
-  </si>
-  <si>
-    <t>Reconocimiento nosotros 2</t>
-  </si>
-  <si>
-    <t>Claridad en ADN: personalidad de mi empresa nosotros 2</t>
-  </si>
-  <si>
-    <t>Liderazgo y trabajo en equipo nosotros 2</t>
-  </si>
-  <si>
-    <t>Rituales nosotros 2</t>
-  </si>
-  <si>
-    <t>Conversaciones nosotros 2</t>
-  </si>
-  <si>
-    <t>Entorno saludable nosotros 2</t>
-  </si>
-  <si>
-    <t>Relevancia nosotros 2</t>
-  </si>
-  <si>
-    <t>Adaptabilidad nosotros 2</t>
-  </si>
-  <si>
-    <t>Toma de decisiones nosotros 2</t>
-  </si>
-  <si>
-    <t>Impacto en la sociedad nosotros 2</t>
-  </si>
-  <si>
-    <t>Empoderamiento nosotros 2</t>
-  </si>
-  <si>
-    <t>Relaciones nosotros 2</t>
-  </si>
-  <si>
-    <t>Conciencia Sostenible nosotros 2</t>
-  </si>
-  <si>
-    <t>Superar metas nosotros 2</t>
-  </si>
-  <si>
-    <t>Equilibrio todos 1</t>
-  </si>
-  <si>
-    <t>Orgullo (eNps) todos 1</t>
-  </si>
-  <si>
-    <t>Pedir ayuda todos 1</t>
-  </si>
-  <si>
-    <t>Reconocimiento todos 1</t>
-  </si>
-  <si>
-    <t>Claridad en ADN: personalidad de mi empresa todos 1</t>
-  </si>
-  <si>
-    <t>Liderazgo y trabajo en equipo todos 1</t>
-  </si>
-  <si>
-    <t>Rituales todos 1</t>
-  </si>
-  <si>
-    <t>Conversaciones todos 1</t>
-  </si>
-  <si>
-    <t>Entorno saludable todos 1</t>
-  </si>
-  <si>
-    <t>Relevancia todos 1</t>
-  </si>
-  <si>
-    <t>Adaptabilidad todos 1</t>
-  </si>
-  <si>
-    <t>Toma de decisiones todos 1</t>
-  </si>
-  <si>
-    <t>Impacto en la sociedad todos 1</t>
-  </si>
-  <si>
-    <t>Empoderamiento todos 1</t>
-  </si>
-  <si>
-    <t>Relaciones todos 1</t>
-  </si>
-  <si>
-    <t>Conciencia Sostenible todos 1</t>
-  </si>
-  <si>
-    <t>Superar metas todos 1</t>
-  </si>
-  <si>
-    <t>Equilibrio todos 2</t>
-  </si>
-  <si>
-    <t>Orgullo (eNps) todos 2</t>
-  </si>
-  <si>
-    <t>Pedir ayuda todos 2</t>
-  </si>
-  <si>
-    <t>Reconocimiento todos 2</t>
-  </si>
-  <si>
-    <t>Claridad en ADN: personalidad de mi empresa todos 2</t>
-  </si>
-  <si>
-    <t>Liderazgo y trabajo en equipo todos 2</t>
-  </si>
-  <si>
-    <t>Rituales todos 2</t>
-  </si>
-  <si>
-    <t>Conversaciones todos 2</t>
-  </si>
-  <si>
-    <t>Entorno saludable todos 2</t>
-  </si>
-  <si>
-    <t>Relevancia todos 2</t>
-  </si>
-  <si>
-    <t>Adaptabilidad todos 2</t>
-  </si>
-  <si>
-    <t>Toma de decisiones todos 2</t>
-  </si>
-  <si>
-    <t>Impacto en la sociedad todos 2</t>
-  </si>
-  <si>
-    <t>Empoderamiento todos 2</t>
-  </si>
-  <si>
-    <t>Relaciones todos 2</t>
-  </si>
-  <si>
-    <t>Conciencia Sostenible todos 2</t>
-  </si>
-  <si>
-    <t>Superar metas todos 2</t>
-  </si>
-  <si>
-    <t>Conexion yo</t>
-  </si>
-  <si>
-    <t>Proposito yo</t>
-  </si>
-  <si>
-    <t>Contribucion yo</t>
-  </si>
-  <si>
-    <t>Retroalimentacion yo</t>
-  </si>
-  <si>
-    <t>Comunicacion yo</t>
-  </si>
-  <si>
-    <t>Contribucion individual a la cultura yo</t>
-  </si>
-  <si>
-    <t>Innovacion yo</t>
-  </si>
-  <si>
-    <t>Conexion nosotros 1</t>
-  </si>
-  <si>
     <t>Tengo claras oportunidades de crecer dentro de mi equipo y de la organizacion</t>
   </si>
   <si>
-    <t>Proposito nosotros 1</t>
-  </si>
-  <si>
-    <t>Contribucion nosotros 1</t>
-  </si>
-  <si>
     <t>Recibo retroalimentacion de mi jefe inmediato que me permite mejorar permanentemente</t>
   </si>
   <si>
-    <t>Retroalimentacion nosotros 1</t>
-  </si>
-  <si>
     <t>Entiendo claramente mi rol y aporte a los resultados del equipo y de la organizacion</t>
   </si>
   <si>
-    <t>Comunicacion nosotros 1</t>
-  </si>
-  <si>
-    <t>Contribucion individual a la cultura nosotros 1</t>
-  </si>
-  <si>
     <t>Tengo libertad para decidir como realizar mi trabajo</t>
   </si>
   <si>
-    <t>Innovacion nosotros 1</t>
-  </si>
-  <si>
     <t>En nuestro equipo le damos mucho valor a la conciencia ecologica y se evidencia en las pequeñas decisiones cotidianas</t>
   </si>
   <si>
-    <t>Conexion nosotros 2</t>
-  </si>
-  <si>
     <t>Tengo acceso a la informacion y recursos necesarios para realizar mi trabajo</t>
   </si>
   <si>
     <t>Mi plan de carrera tiene futuro si permanezco en esta organizacion</t>
   </si>
   <si>
-    <t>Proposito nosotros 2</t>
-  </si>
-  <si>
     <t>Mi relacion con mi jefe inmediato se basa en el respeto y la claridad</t>
   </si>
   <si>
     <t>En el equipo cada uno sabe su tarea y es fundamental favorecer su concentracion para que la logre</t>
   </si>
   <si>
-    <t>Contribucion nosotros 2</t>
-  </si>
-  <si>
-    <t>Retroalimentacion nosotros 2</t>
-  </si>
-  <si>
     <t>La comunicacion del equipo nos acerca como personas y facilita nuestros resultados</t>
   </si>
   <si>
-    <t>Comunicacion nosotros 2</t>
-  </si>
-  <si>
-    <t>Contribucion individual a la cultura nosotros 2</t>
-  </si>
-  <si>
-    <t>Innovacion nosotros 2</t>
-  </si>
-  <si>
-    <t>Conexion todos 1</t>
-  </si>
-  <si>
     <t>La organizacion propicia un sano equilibrio vida/trabajo</t>
   </si>
   <si>
     <t>El proposito de la organizacion me impulsa y saca lo mejor de mi</t>
   </si>
   <si>
-    <t>Proposito todos 1</t>
-  </si>
-  <si>
     <t>Me siento orgulloso de ser parte del equipo humano de esta organizacion</t>
   </si>
   <si>
@@ -1293,12 +963,6 @@
     <t>En la organizacion todos contribuimos de manera destacada</t>
   </si>
   <si>
-    <t>Contribucion todos 1</t>
-  </si>
-  <si>
-    <t>Retroalimentacion todos 1</t>
-  </si>
-  <si>
     <t>Mis resultados son reconocidos y valorados por la organizacion</t>
   </si>
   <si>
@@ -1308,21 +972,12 @@
     <t>Somos una organizacion con buena comunicacion: escuchamos y somos escuchados y sabemos lo que pasa</t>
   </si>
   <si>
-    <t>Comunicacion todos 1</t>
-  </si>
-  <si>
     <t>Las personas que trabajan en la organizacion imprimen sus propias cualidades en la cultura y la enriquecen</t>
   </si>
   <si>
-    <t>Contribucion individual a la cultura todos 1</t>
-  </si>
-  <si>
     <t>En esta organizacion los espacios para conversar y escuchar son frecuentes y valorados</t>
   </si>
   <si>
-    <t>Innovacion todos 1</t>
-  </si>
-  <si>
     <t>Los espacios de esta organizacion son excepcionales</t>
   </si>
   <si>
@@ -1347,45 +1002,24 @@
     <t>Me inspira la mision y proposito de la organizacion</t>
   </si>
   <si>
-    <t>Conexion todos 2</t>
-  </si>
-  <si>
     <t>Los planes y proyectos nuevos de la organizacion se acompasan y conectan con el ritmo del equipo y sus planes previamente trazados</t>
   </si>
   <si>
-    <t>Proposito todos 2</t>
-  </si>
-  <si>
     <t>Pedir ayuda es poco habitual en nuestra organizacion</t>
   </si>
   <si>
     <t>En la organizacion tengo la oportunidad de mejorar mis habilidades</t>
   </si>
   <si>
-    <t>Contribucion todos 2</t>
-  </si>
-  <si>
-    <t>Retroalimentacion todos 2</t>
-  </si>
-  <si>
     <t>La imagen que se percibe de la organizacion se corresponde con lo que yo vivo como colaborador</t>
   </si>
   <si>
     <t>Tenemos serios problemas de comunicacion: no tenemos espacios para escucharnos y no siempre nos enteramos de lo que pasa</t>
   </si>
   <si>
-    <t>Comunicacion todos 2</t>
-  </si>
-  <si>
-    <t>Contribucion individual a la cultura todos 2</t>
-  </si>
-  <si>
     <t>Me siento comodo en esta cultura y entorno organizacional</t>
   </si>
   <si>
-    <t>Innovacion todos 2</t>
-  </si>
-  <si>
     <t>Los espacios de la organizacion son confortable y me aporta lo que necesito para estar bien</t>
   </si>
   <si>
@@ -1431,30 +1065,18 @@
     <t>Se que hace cada persona de mi equipo. Les puedo ayudar y puedo contar con mis pares cuando necesito ayuda</t>
   </si>
   <si>
-    <t>Espacios fisicos aliados de la cultura yo</t>
-  </si>
-  <si>
-    <t>Servir con cercania yo</t>
-  </si>
-  <si>
     <t>En nuestro equipo todos aportamos y el lider nos acompaña y direcciona para lograr resultados superiores a los esperados</t>
   </si>
   <si>
     <t>Con mi equipo inmediato me siento en un entorno saludable fisica y emocionalmente</t>
   </si>
   <si>
-    <t>Espacios fisicos aliados de la cultura nosotros 1</t>
-  </si>
-  <si>
     <t>Mi jefe es justo, claro y profesional para tomar decisiones. Confio en su criterio</t>
   </si>
   <si>
     <t>Siento el respaldo de mi lider, incluso cuando cometo errores</t>
   </si>
   <si>
-    <t>Servir con cercania nosotros 1</t>
-  </si>
-  <si>
     <t>Mi lider es claro con las metas y despliega incentivos claros para motivar resultados mas alla de lo esperado</t>
   </si>
   <si>
@@ -1464,33 +1086,15 @@
     <t>Yo me aseguro de no ser un problema para los demas. Otros deberian hacer lo mismo</t>
   </si>
   <si>
-    <t>Espacios fisicos aliados de la cultura nosotros 2</t>
-  </si>
-  <si>
     <t>El lider es claro y asigna las tareas a cada persona para lograr los objetivos del equipo</t>
   </si>
   <si>
-    <t>Servir con cercania nosotros 2</t>
-  </si>
-  <si>
-    <t>Espacios fisicos aliados de la cultura todos 1</t>
-  </si>
-  <si>
-    <t>Servir con cercania todos 1</t>
-  </si>
-  <si>
     <t>Mi familia y amigos se sienten orgullosos de que yo trabaje aqui</t>
   </si>
   <si>
     <t>Trabajar aqui me hace sentir bienestar. Me siento protegido y tranquilo</t>
   </si>
   <si>
-    <t>Espacios fisicos aliados de la cultura todos 2</t>
-  </si>
-  <si>
-    <t>Servir con cercania todos 2</t>
-  </si>
-  <si>
     <t>Los valores que promueve la organizacion corresponden con los mios</t>
   </si>
   <si>
@@ -1534,6 +1138,102 @@
   </si>
   <si>
     <t>Las decisiones que ha tomado la organizacion en el ultimo año nos llevaran mas lejos y estan alineadas a los objetivos</t>
+  </si>
+  <si>
+    <t>nivel</t>
+  </si>
+  <si>
+    <t>yo</t>
+  </si>
+  <si>
+    <t>nosotros 1</t>
+  </si>
+  <si>
+    <t>nosotros 2</t>
+  </si>
+  <si>
+    <t>todos 1</t>
+  </si>
+  <si>
+    <t>todos 2</t>
+  </si>
+  <si>
+    <t>Conexion</t>
+  </si>
+  <si>
+    <t>Equilibrio</t>
+  </si>
+  <si>
+    <t>Proposito</t>
+  </si>
+  <si>
+    <t>Orgullo (eNps)</t>
+  </si>
+  <si>
+    <t>Pedir ayuda</t>
+  </si>
+  <si>
+    <t>Contribucion</t>
+  </si>
+  <si>
+    <t>Retroalimentacion</t>
+  </si>
+  <si>
+    <t>Reconocimiento</t>
+  </si>
+  <si>
+    <t>Claridad en ADN: personalidad de mi empresa</t>
+  </si>
+  <si>
+    <t>Liderazgo y trabajo en equipo</t>
+  </si>
+  <si>
+    <t>Rituales</t>
+  </si>
+  <si>
+    <t>Comunicacion</t>
+  </si>
+  <si>
+    <t>Contribucion individual a la cultura</t>
+  </si>
+  <si>
+    <t>Conversaciones</t>
+  </si>
+  <si>
+    <t>Entorno saludable</t>
+  </si>
+  <si>
+    <t>Relevancia</t>
+  </si>
+  <si>
+    <t>Innovacion</t>
+  </si>
+  <si>
+    <t>Espacios fisicos aliados de la cultura</t>
+  </si>
+  <si>
+    <t>Adaptabilidad</t>
+  </si>
+  <si>
+    <t>Toma de decisiones</t>
+  </si>
+  <si>
+    <t>Impacto en la sociedad</t>
+  </si>
+  <si>
+    <t>Empoderamiento</t>
+  </si>
+  <si>
+    <t>Relaciones</t>
+  </si>
+  <si>
+    <t>Conciencia Sostenible</t>
+  </si>
+  <si>
+    <t>Servir con cercania</t>
+  </si>
+  <si>
+    <t>Superar metas</t>
   </si>
 </sst>
 </file>
@@ -1966,19 +1666,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224B91BE-E32E-4506-A86E-9E3F6E02D172}">
-  <dimension ref="A1:E131"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.375" customWidth="1"/>
     <col min="2" max="2" width="53.875" customWidth="1"/>
+    <col min="4" max="4" width="48.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>33</v>
       </c>
@@ -1994,450 +1695,531 @@
       <c r="E1" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="E2" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>296</v>
+        <v>377</v>
       </c>
       <c r="E3" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E4" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>297</v>
+        <v>379</v>
       </c>
       <c r="E5" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C6" s="1">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>298</v>
+        <v>380</v>
       </c>
       <c r="E6" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E7" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C8" s="1">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E8" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>299</v>
+        <v>383</v>
       </c>
       <c r="E9" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C10" s="1">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>300</v>
+        <v>384</v>
       </c>
       <c r="E10" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C11" s="1">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>301</v>
+        <v>385</v>
       </c>
       <c r="E11" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C12" s="1">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>302</v>
+        <v>386</v>
       </c>
       <c r="E12" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="E13" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="E14" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>303</v>
+        <v>389</v>
       </c>
       <c r="E15" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>304</v>
+        <v>390</v>
       </c>
       <c r="E16" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>305</v>
+        <v>391</v>
       </c>
       <c r="E17" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="E18" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>465</v>
+        <v>393</v>
       </c>
       <c r="E19" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>306</v>
+        <v>394</v>
       </c>
       <c r="E20" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C21" s="1">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>307</v>
+        <v>395</v>
       </c>
       <c r="E21" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>308</v>
+        <v>396</v>
       </c>
       <c r="E22" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>309</v>
+        <v>397</v>
       </c>
       <c r="E23" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C24" s="1">
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>310</v>
+        <v>398</v>
       </c>
       <c r="E24" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C25" s="1">
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>311</v>
+        <v>399</v>
       </c>
       <c r="E25" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C26" s="1">
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>466</v>
+        <v>400</v>
       </c>
       <c r="E26" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>457</v>
+        <v>337</v>
       </c>
       <c r="C27" s="1">
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>312</v>
+        <v>401</v>
       </c>
       <c r="E27" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>60</v>
       </c>
@@ -2448,47 +2230,56 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="E28" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>458</v>
+        <v>338</v>
       </c>
       <c r="C29" s="1">
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>313</v>
+        <v>377</v>
       </c>
       <c r="E29" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>389</v>
+        <v>296</v>
       </c>
       <c r="C30" s="1">
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="E30" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F30" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>63</v>
       </c>
@@ -2499,13 +2290,16 @@
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>314</v>
+        <v>379</v>
       </c>
       <c r="E31" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>64</v>
       </c>
@@ -2516,13 +2310,16 @@
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>315</v>
+        <v>380</v>
       </c>
       <c r="E32" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>65</v>
       </c>
@@ -2533,30 +2330,36 @@
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="E33" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>392</v>
+        <v>297</v>
       </c>
       <c r="C34" s="1">
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="E34" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>67</v>
       </c>
@@ -2567,47 +2370,56 @@
         <v>#N/A</v>
       </c>
       <c r="D35" t="s">
-        <v>316</v>
+        <v>383</v>
       </c>
       <c r="E35" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F35" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>394</v>
+        <v>298</v>
       </c>
       <c r="C36" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D36" t="s">
-        <v>317</v>
+        <v>384</v>
       </c>
       <c r="E36" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>467</v>
+        <v>345</v>
       </c>
       <c r="C37" s="1">
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>318</v>
+        <v>385</v>
       </c>
       <c r="E37" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F37" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>70</v>
       </c>
@@ -2618,13 +2430,16 @@
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>319</v>
+        <v>386</v>
       </c>
       <c r="E38" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F38" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>71</v>
       </c>
@@ -2635,13 +2450,16 @@
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="E39" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F39" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>72</v>
       </c>
@@ -2652,13 +2470,16 @@
         <v>#N/A</v>
       </c>
       <c r="D40" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="E40" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F40" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>73</v>
       </c>
@@ -2669,64 +2490,76 @@
         <v>#N/A</v>
       </c>
       <c r="D41" t="s">
-        <v>320</v>
+        <v>389</v>
       </c>
       <c r="E41" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F41" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>468</v>
+        <v>346</v>
       </c>
       <c r="C42" s="1">
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>321</v>
+        <v>390</v>
       </c>
       <c r="E42" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F42" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>397</v>
+        <v>299</v>
       </c>
       <c r="C43" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D43" t="s">
-        <v>322</v>
+        <v>391</v>
       </c>
       <c r="E43" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F43" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>459</v>
+        <v>339</v>
       </c>
       <c r="C44" s="1">
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="E44" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F44" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>77</v>
       </c>
@@ -2737,13 +2570,16 @@
         <v>#N/A</v>
       </c>
       <c r="D45" t="s">
-        <v>469</v>
+        <v>393</v>
       </c>
       <c r="E45" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F45" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>78</v>
       </c>
@@ -2754,30 +2590,36 @@
         <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>323</v>
+        <v>394</v>
       </c>
       <c r="E46" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F46" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>470</v>
+        <v>347</v>
       </c>
       <c r="C47" s="1">
         <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>324</v>
+        <v>395</v>
       </c>
       <c r="E47" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F47" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>80</v>
       </c>
@@ -2788,13 +2630,16 @@
         <v>#N/A</v>
       </c>
       <c r="D48" t="s">
-        <v>325</v>
+        <v>396</v>
       </c>
       <c r="E48" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F48" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>81</v>
       </c>
@@ -2805,13 +2650,16 @@
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>326</v>
+        <v>397</v>
       </c>
       <c r="E49" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F49" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>82</v>
       </c>
@@ -2822,64 +2670,76 @@
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>327</v>
+        <v>398</v>
       </c>
       <c r="E50" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F50" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>399</v>
+        <v>300</v>
       </c>
       <c r="C51" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D51" t="s">
-        <v>328</v>
+        <v>399</v>
       </c>
       <c r="E51" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F51" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>471</v>
+        <v>348</v>
       </c>
       <c r="C52" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D52" t="s">
-        <v>472</v>
+        <v>400</v>
       </c>
       <c r="E52" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F52" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>473</v>
+        <v>349</v>
       </c>
       <c r="C53" s="1">
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>329</v>
+        <v>401</v>
       </c>
       <c r="E53" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F53" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>86</v>
       </c>
@@ -2890,115 +2750,136 @@
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>400</v>
+        <v>376</v>
       </c>
       <c r="E54" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F54" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>401</v>
+        <v>301</v>
       </c>
       <c r="C55" s="1">
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>330</v>
+        <v>377</v>
       </c>
       <c r="E55" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F55" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>402</v>
+        <v>302</v>
       </c>
       <c r="C56" s="1">
         <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>403</v>
+        <v>378</v>
       </c>
       <c r="E56" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F56" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>404</v>
+        <v>303</v>
       </c>
       <c r="C57" s="1">
         <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>331</v>
+        <v>379</v>
       </c>
       <c r="E57" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F57" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>405</v>
+        <v>304</v>
       </c>
       <c r="C58" s="1">
         <v>0</v>
       </c>
       <c r="D58" t="s">
-        <v>332</v>
+        <v>380</v>
       </c>
       <c r="E58" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F58" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>460</v>
+        <v>340</v>
       </c>
       <c r="C59" s="1">
         <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>406</v>
+        <v>381</v>
       </c>
       <c r="E59" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F59" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>461</v>
+        <v>341</v>
       </c>
       <c r="C60" s="1">
         <v>0</v>
       </c>
       <c r="D60" t="s">
-        <v>407</v>
+        <v>382</v>
       </c>
       <c r="E60" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F60" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>93</v>
       </c>
@@ -3009,13 +2890,16 @@
         <v>0</v>
       </c>
       <c r="D61" t="s">
-        <v>333</v>
+        <v>383</v>
       </c>
       <c r="E61" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F61" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>94</v>
       </c>
@@ -3026,13 +2910,16 @@
         <v>#N/A</v>
       </c>
       <c r="D62" t="s">
-        <v>334</v>
+        <v>384</v>
       </c>
       <c r="E62" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F62" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>95</v>
       </c>
@@ -3043,47 +2930,56 @@
         <v>#N/A</v>
       </c>
       <c r="D63" t="s">
-        <v>335</v>
+        <v>385</v>
       </c>
       <c r="E63" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F63" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>474</v>
+        <v>350</v>
       </c>
       <c r="C64" s="1">
         <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>336</v>
+        <v>386</v>
       </c>
       <c r="E64" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F64" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>408</v>
+        <v>305</v>
       </c>
       <c r="C65" s="1">
         <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>409</v>
+        <v>387</v>
       </c>
       <c r="E65" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F65" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>98</v>
       </c>
@@ -3094,13 +2990,16 @@
         <v>#N/A</v>
       </c>
       <c r="D66" t="s">
-        <v>410</v>
+        <v>388</v>
       </c>
       <c r="E66" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F66" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>99</v>
       </c>
@@ -3111,64 +3010,76 @@
         <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>337</v>
+        <v>389</v>
       </c>
       <c r="E67" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F67" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>475</v>
+        <v>351</v>
       </c>
       <c r="C68" s="1">
         <v>0</v>
       </c>
       <c r="D68" t="s">
-        <v>338</v>
+        <v>390</v>
       </c>
       <c r="E68" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F68" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>462</v>
+        <v>342</v>
       </c>
       <c r="C69" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D69" t="s">
-        <v>339</v>
+        <v>391</v>
       </c>
       <c r="E69" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F69" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>463</v>
+        <v>343</v>
       </c>
       <c r="C70" s="1">
         <v>1</v>
       </c>
       <c r="D70" t="s">
-        <v>411</v>
+        <v>392</v>
       </c>
       <c r="E70" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F70" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>103</v>
       </c>
@@ -3179,13 +3090,16 @@
         <v>#N/A</v>
       </c>
       <c r="D71" t="s">
-        <v>476</v>
+        <v>393</v>
       </c>
       <c r="E71" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F71" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>104</v>
       </c>
@@ -3196,30 +3110,36 @@
         <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>340</v>
+        <v>394</v>
       </c>
       <c r="E72" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F72" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>464</v>
+        <v>344</v>
       </c>
       <c r="C73" s="1">
         <v>0</v>
       </c>
       <c r="D73" t="s">
-        <v>341</v>
+        <v>395</v>
       </c>
       <c r="E73" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F73" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>106</v>
       </c>
@@ -3230,30 +3150,36 @@
         <v>#N/A</v>
       </c>
       <c r="D74" t="s">
-        <v>342</v>
+        <v>396</v>
       </c>
       <c r="E74" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F74" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>477</v>
+        <v>352</v>
       </c>
       <c r="C75" s="1">
         <v>0</v>
       </c>
       <c r="D75" t="s">
-        <v>343</v>
+        <v>397</v>
       </c>
       <c r="E75" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F75" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>108</v>
       </c>
@@ -3264,13 +3190,16 @@
         <v>0</v>
       </c>
       <c r="D76" t="s">
-        <v>344</v>
+        <v>398</v>
       </c>
       <c r="E76" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F76" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>109</v>
       </c>
@@ -3281,13 +3210,16 @@
         <v>#N/A</v>
       </c>
       <c r="D77" t="s">
-        <v>345</v>
+        <v>399</v>
       </c>
       <c r="E77" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F77" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>110</v>
       </c>
@@ -3298,13 +3230,16 @@
         <v>#N/A</v>
       </c>
       <c r="D78" t="s">
-        <v>478</v>
+        <v>400</v>
       </c>
       <c r="E78" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F78" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>111</v>
       </c>
@@ -3315,268 +3250,316 @@
         <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>346</v>
+        <v>401</v>
       </c>
       <c r="E79" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F79" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>485</v>
+        <v>355</v>
       </c>
       <c r="C80" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D80" t="s">
-        <v>412</v>
+        <v>376</v>
       </c>
       <c r="E80" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F80" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>413</v>
+        <v>306</v>
       </c>
       <c r="C81" s="1">
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>347</v>
+        <v>377</v>
       </c>
       <c r="E81" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F81" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>414</v>
+        <v>307</v>
       </c>
       <c r="C82" s="1">
         <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>415</v>
+        <v>378</v>
       </c>
       <c r="E82" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F82" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>416</v>
+        <v>308</v>
       </c>
       <c r="C83" s="1">
         <v>0</v>
       </c>
       <c r="D83" t="s">
-        <v>348</v>
+        <v>379</v>
       </c>
       <c r="E83" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F83" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>417</v>
+        <v>309</v>
       </c>
       <c r="C84" s="1">
         <v>0</v>
       </c>
       <c r="D84" t="s">
-        <v>349</v>
+        <v>380</v>
       </c>
       <c r="E84" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F84" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>418</v>
+        <v>310</v>
       </c>
       <c r="C85" s="1">
         <v>0</v>
       </c>
       <c r="D85" t="s">
-        <v>419</v>
+        <v>381</v>
       </c>
       <c r="E85" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F85" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>486</v>
+        <v>356</v>
       </c>
       <c r="C86" s="1">
         <v>0</v>
       </c>
       <c r="D86" t="s">
-        <v>420</v>
+        <v>382</v>
       </c>
       <c r="E86" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F86" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>421</v>
+        <v>311</v>
       </c>
       <c r="C87" s="1">
         <v>0</v>
       </c>
       <c r="D87" t="s">
-        <v>350</v>
+        <v>383</v>
       </c>
       <c r="E87" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F87" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>487</v>
+        <v>357</v>
       </c>
       <c r="C88" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D88" t="s">
-        <v>351</v>
+        <v>384</v>
       </c>
       <c r="E88" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F88" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>488</v>
+        <v>358</v>
       </c>
       <c r="C89" s="1">
         <v>0</v>
       </c>
       <c r="D89" t="s">
-        <v>352</v>
+        <v>385</v>
       </c>
       <c r="E89" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F89" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>422</v>
+        <v>312</v>
       </c>
       <c r="C90" s="1">
         <v>0</v>
       </c>
       <c r="D90" t="s">
-        <v>353</v>
+        <v>386</v>
       </c>
       <c r="E90" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F90" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>123</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>423</v>
+        <v>313</v>
       </c>
       <c r="C91" s="1">
         <v>0</v>
       </c>
       <c r="D91" t="s">
-        <v>424</v>
+        <v>387</v>
       </c>
       <c r="E91" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F91" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>425</v>
+        <v>314</v>
       </c>
       <c r="C92" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D92" t="s">
-        <v>426</v>
+        <v>388</v>
       </c>
       <c r="E92" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F92" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>427</v>
+        <v>315</v>
       </c>
       <c r="C93" s="1">
         <v>0</v>
       </c>
       <c r="D93" t="s">
-        <v>354</v>
+        <v>389</v>
       </c>
       <c r="E93" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F93" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>489</v>
+        <v>359</v>
       </c>
       <c r="C94" s="1">
         <v>0</v>
       </c>
       <c r="D94" t="s">
-        <v>355</v>
+        <v>390</v>
       </c>
       <c r="E94" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F94" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>127</v>
       </c>
@@ -3587,302 +3570,356 @@
         <v>#N/A</v>
       </c>
       <c r="D95" t="s">
-        <v>356</v>
+        <v>391</v>
       </c>
       <c r="E95" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F95" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>490</v>
+        <v>360</v>
       </c>
       <c r="C96" s="1">
         <v>0</v>
       </c>
       <c r="D96" t="s">
-        <v>428</v>
+        <v>392</v>
       </c>
       <c r="E96" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F96" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>429</v>
+        <v>316</v>
       </c>
       <c r="C97" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D97" t="s">
-        <v>479</v>
+        <v>393</v>
       </c>
       <c r="E97" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F97" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>130</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>430</v>
+        <v>317</v>
       </c>
       <c r="C98" s="1">
         <v>0</v>
       </c>
       <c r="D98" t="s">
-        <v>357</v>
+        <v>394</v>
       </c>
       <c r="E98" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F98" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>499</v>
+        <v>369</v>
       </c>
       <c r="C99" s="1">
         <v>0</v>
       </c>
       <c r="D99" t="s">
-        <v>358</v>
+        <v>395</v>
       </c>
       <c r="E99" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F99" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>431</v>
+        <v>318</v>
       </c>
       <c r="C100" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D100" t="s">
-        <v>359</v>
+        <v>396</v>
       </c>
       <c r="E100" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F100" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>133</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>432</v>
+        <v>319</v>
       </c>
       <c r="C101" s="1">
         <v>0</v>
       </c>
       <c r="D101" t="s">
-        <v>360</v>
+        <v>397</v>
       </c>
       <c r="E101" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F101" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>134</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>433</v>
+        <v>320</v>
       </c>
       <c r="C102" s="1">
         <v>0</v>
       </c>
       <c r="D102" t="s">
-        <v>361</v>
+        <v>398</v>
       </c>
       <c r="E102" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F102" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>491</v>
+        <v>361</v>
       </c>
       <c r="C103" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D103" t="s">
-        <v>362</v>
+        <v>399</v>
       </c>
       <c r="E103" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F103" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>136</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>434</v>
+        <v>321</v>
       </c>
       <c r="C104" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D104" t="s">
-        <v>480</v>
+        <v>400</v>
       </c>
       <c r="E104" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F104" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>435</v>
+        <v>322</v>
       </c>
       <c r="C105" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D105" t="s">
-        <v>363</v>
+        <v>401</v>
       </c>
       <c r="E105" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F105" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>138</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>436</v>
+        <v>323</v>
       </c>
       <c r="C106" s="1">
         <v>0</v>
       </c>
       <c r="D106" t="s">
-        <v>437</v>
+        <v>376</v>
       </c>
       <c r="E106" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F106" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>139</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>438</v>
+        <v>324</v>
       </c>
       <c r="C107" s="1">
         <v>0</v>
       </c>
       <c r="D107" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="E107" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F107" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>492</v>
+        <v>362</v>
       </c>
       <c r="C108" s="1">
         <v>0</v>
       </c>
       <c r="D108" t="s">
-        <v>439</v>
+        <v>378</v>
       </c>
       <c r="E108" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F108" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>141</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>481</v>
+        <v>353</v>
       </c>
       <c r="C109" s="1">
         <v>0</v>
       </c>
       <c r="D109" t="s">
-        <v>365</v>
+        <v>379</v>
       </c>
       <c r="E109" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F109" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>142</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>440</v>
+        <v>325</v>
       </c>
       <c r="C110" s="1">
         <v>1</v>
       </c>
       <c r="D110" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
       <c r="E110" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F110" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>143</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>441</v>
+        <v>326</v>
       </c>
       <c r="C111" s="1">
         <v>0</v>
       </c>
       <c r="D111" t="s">
-        <v>442</v>
+        <v>381</v>
       </c>
       <c r="E111" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F111" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>144</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>493</v>
+        <v>363</v>
       </c>
       <c r="C112" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D112" t="s">
-        <v>443</v>
+        <v>382</v>
       </c>
       <c r="E112" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F112" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>145</v>
       </c>
@@ -3893,30 +3930,36 @@
         <v>#N/A</v>
       </c>
       <c r="D113" t="s">
-        <v>367</v>
+        <v>383</v>
       </c>
       <c r="E113" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F113" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>146</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>444</v>
+        <v>327</v>
       </c>
       <c r="C114" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D114" t="s">
-        <v>368</v>
+        <v>384</v>
       </c>
       <c r="E114" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F114" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>147</v>
       </c>
@@ -3927,13 +3970,16 @@
         <v>0</v>
       </c>
       <c r="D115" t="s">
-        <v>369</v>
+        <v>385</v>
       </c>
       <c r="E115" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F115" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>148</v>
       </c>
@@ -3944,265 +3990,313 @@
         <v>0</v>
       </c>
       <c r="D116" t="s">
-        <v>370</v>
+        <v>386</v>
       </c>
       <c r="E116" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F116" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>149</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>445</v>
+        <v>328</v>
       </c>
       <c r="C117" s="1">
         <v>1</v>
       </c>
       <c r="D117" t="s">
-        <v>446</v>
+        <v>387</v>
       </c>
       <c r="E117" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F117" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>150</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>494</v>
+        <v>364</v>
       </c>
       <c r="C118" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D118" t="s">
-        <v>447</v>
+        <v>388</v>
       </c>
       <c r="E118" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F118" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>151</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>495</v>
+        <v>365</v>
       </c>
       <c r="C119" s="1">
         <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>371</v>
+        <v>389</v>
       </c>
       <c r="E119" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F119" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>152</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>482</v>
+        <v>354</v>
       </c>
       <c r="C120" s="1">
         <v>0</v>
       </c>
       <c r="D120" t="s">
-        <v>372</v>
+        <v>390</v>
       </c>
       <c r="E120" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F120" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>153</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>448</v>
+        <v>329</v>
       </c>
       <c r="C121" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D121" t="s">
-        <v>373</v>
+        <v>391</v>
       </c>
       <c r="E121" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F121" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>154</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>496</v>
+        <v>366</v>
       </c>
       <c r="C122" s="1">
         <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>449</v>
+        <v>392</v>
       </c>
       <c r="E122" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F122" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>155</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>450</v>
+        <v>330</v>
       </c>
       <c r="C123" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D123" t="s">
-        <v>483</v>
+        <v>393</v>
       </c>
       <c r="E123" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F123" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>156</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>451</v>
+        <v>331</v>
       </c>
       <c r="C124" s="1">
         <v>1</v>
       </c>
       <c r="D124" t="s">
-        <v>374</v>
+        <v>394</v>
       </c>
       <c r="E124" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F124" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>157</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>452</v>
+        <v>332</v>
       </c>
       <c r="C125" s="1">
         <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>375</v>
+        <v>395</v>
       </c>
       <c r="E125" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F125" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>158</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>453</v>
+        <v>333</v>
       </c>
       <c r="C126" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D126" t="s">
-        <v>376</v>
+        <v>396</v>
       </c>
       <c r="E126" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F126" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>159</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>497</v>
+        <v>367</v>
       </c>
       <c r="C127" s="1">
         <v>0</v>
       </c>
       <c r="D127" t="s">
-        <v>377</v>
+        <v>397</v>
       </c>
       <c r="E127" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F127" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>160</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>454</v>
+        <v>334</v>
       </c>
       <c r="C128" s="1">
         <v>0</v>
       </c>
       <c r="D128" t="s">
-        <v>378</v>
+        <v>398</v>
       </c>
       <c r="E128" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F128" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>161</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>455</v>
+        <v>335</v>
       </c>
       <c r="C129" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D129" t="s">
-        <v>379</v>
+        <v>399</v>
       </c>
       <c r="E129" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F129" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>162</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>456</v>
+        <v>336</v>
       </c>
       <c r="C130" s="1" t="e">
         <v>#N/A</v>
       </c>
       <c r="D130" t="s">
-        <v>484</v>
+        <v>400</v>
       </c>
       <c r="E130" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F130" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>163</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>498</v>
+        <v>368</v>
       </c>
       <c r="C131" s="1">
         <v>0</v>
       </c>
       <c r="D131" t="s">
-        <v>380</v>
+        <v>401</v>
       </c>
       <c r="E131" t="s">
         <v>294</v>
+      </c>
+      <c r="F131" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>